<commit_message>
avances en codigos aduaneros
</commit_message>
<xml_diff>
--- a/information/raw_databases/ADUANAS_CHILE/arancel_aduanero_nomenclatura/arancel_aduanero_2017/codigos_aduana_por_especie_2017.xlsx
+++ b/information/raw_databases/ADUANAS_CHILE/arancel_aduanero_nomenclatura/arancel_aduanero_2017/codigos_aduana_por_especie_2017.xlsx
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="781">
   <si>
     <t>especie_SERNAPESCA</t>
   </si>
@@ -2318,13 +2318,241 @@
   </si>
   <si>
     <t>0305.7123</t>
+  </si>
+  <si>
+    <t>0301.9100</t>
+  </si>
+  <si>
+    <t>0302.11</t>
+  </si>
+  <si>
+    <t>0303.14</t>
+  </si>
+  <si>
+    <t>0303.1410</t>
+  </si>
+  <si>
+    <t>0303.1420</t>
+  </si>
+  <si>
+    <t>0303.1430</t>
+  </si>
+  <si>
+    <t>0303.1440</t>
+  </si>
+  <si>
+    <t>0303.1490</t>
+  </si>
+  <si>
+    <t>0304.4200</t>
+  </si>
+  <si>
+    <t>0304.8200</t>
+  </si>
+  <si>
+    <t>0304.9951</t>
+  </si>
+  <si>
+    <t>0304.9959</t>
+  </si>
+  <si>
+    <t>0305.2020</t>
+  </si>
+  <si>
+    <t>0305.3920</t>
+  </si>
+  <si>
+    <t>0305.43</t>
+  </si>
+  <si>
+    <t>0305.4310</t>
+  </si>
+  <si>
+    <t>0305.4320</t>
+  </si>
+  <si>
+    <t>0305.4330</t>
+  </si>
+  <si>
+    <t>0305.4390</t>
+  </si>
+  <si>
+    <t>Psetta maxima</t>
+  </si>
+  <si>
+    <t>0302.2400</t>
+  </si>
+  <si>
+    <t>0303.3400</t>
+  </si>
+  <si>
+    <t>0307.8110</t>
+  </si>
+  <si>
+    <t>0307.8320</t>
+  </si>
+  <si>
+    <t>1605.5710</t>
+  </si>
+  <si>
+    <t>0307.8310</t>
+  </si>
+  <si>
+    <t>Ameghinomya antiqua</t>
+  </si>
+  <si>
+    <t>0307.7110</t>
+  </si>
+  <si>
+    <t>0307.7211</t>
+  </si>
+  <si>
+    <t>1605.5611</t>
+  </si>
+  <si>
+    <t>0307.4220</t>
+  </si>
+  <si>
+    <t>Loligo spp</t>
+  </si>
+  <si>
+    <t>0307.9224</t>
+  </si>
+  <si>
+    <t>1605.5934</t>
+  </si>
+  <si>
+    <t>0307.9223</t>
+  </si>
+  <si>
+    <t>1605.5933</t>
+  </si>
+  <si>
+    <t>0307.9221</t>
+  </si>
+  <si>
+    <t>1605.5931</t>
+  </si>
+  <si>
+    <t>Trophon gervesianus</t>
+  </si>
+  <si>
+    <t>0307.9222</t>
+  </si>
+  <si>
+    <t>1605.5932</t>
+  </si>
+  <si>
+    <t>1605.5300</t>
+  </si>
+  <si>
+    <t>Mytilus spp.</t>
+  </si>
+  <si>
+    <t>0307.3100</t>
+  </si>
+  <si>
+    <t>0307.3200</t>
+  </si>
+  <si>
+    <t>0307.3900</t>
+  </si>
+  <si>
+    <t>1605.5970</t>
+  </si>
+  <si>
+    <t>0307.7120</t>
+  </si>
+  <si>
+    <t>0307.7215</t>
+  </si>
+  <si>
+    <t>1605.5960</t>
+  </si>
+  <si>
+    <t>0307.4320</t>
+  </si>
+  <si>
+    <t>0307.4330</t>
+  </si>
+  <si>
+    <t>0307.4340</t>
+  </si>
+  <si>
+    <t>0307.7212</t>
+  </si>
+  <si>
+    <t>1605.5612</t>
+  </si>
+  <si>
+    <t>0307.9230</t>
+  </si>
+  <si>
+    <t>0307.9130</t>
+  </si>
+  <si>
+    <t>0307.9210</t>
+  </si>
+  <si>
+    <t>1605.5920</t>
+  </si>
+  <si>
+    <t>0307.7213</t>
+  </si>
+  <si>
+    <t>1605.5910</t>
+  </si>
+  <si>
+    <t>0307.7216</t>
+  </si>
+  <si>
+    <t>1605.5950</t>
+  </si>
+  <si>
+    <t>0307.2110</t>
+  </si>
+  <si>
+    <t>0307.2210</t>
+  </si>
+  <si>
+    <t>0307.2910</t>
+  </si>
+  <si>
+    <t>1605.5210</t>
+  </si>
+  <si>
+    <t>0307.2120</t>
+  </si>
+  <si>
+    <t>0307.2220</t>
+  </si>
+  <si>
+    <t>0307.2920</t>
+  </si>
+  <si>
+    <t>0307.1110</t>
+  </si>
+  <si>
+    <t>0307.1210</t>
+  </si>
+  <si>
+    <t>Crassostrea gigas</t>
+  </si>
+  <si>
+    <t>0307.1120</t>
+  </si>
+  <si>
+    <t>0307.1220</t>
+  </si>
+  <si>
+    <t>1605.5100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2378,6 +2606,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2402,8 +2637,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -2421,12 +2662,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2739,11 +2986,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G472"/>
+  <dimension ref="A1:G521"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A350" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C356" sqref="C356"/>
+      <pane ySplit="1" topLeftCell="A420" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D445" sqref="D445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7465,7 +7712,7 @@
         <v>1</v>
       </c>
       <c r="F205">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G205">
         <v>0</v>
@@ -7488,7 +7735,7 @@
         <v>1</v>
       </c>
       <c r="F206">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G206">
         <v>0</v>
@@ -7879,7 +8126,7 @@
         <v>1</v>
       </c>
       <c r="F223">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G223">
         <v>0</v>
@@ -7902,7 +8149,7 @@
         <v>1</v>
       </c>
       <c r="F224">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G224">
         <v>0</v>
@@ -9282,7 +9529,7 @@
         <v>1</v>
       </c>
       <c r="F284">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G284">
         <v>0</v>
@@ -9305,7 +9552,7 @@
         <v>1</v>
       </c>
       <c r="F285">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G285">
         <v>0</v>
@@ -9328,7 +9575,7 @@
         <v>1</v>
       </c>
       <c r="F286">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G286">
         <v>0</v>
@@ -9351,7 +9598,7 @@
         <v>1</v>
       </c>
       <c r="F287">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G287">
         <v>0</v>
@@ -9374,7 +9621,7 @@
         <v>1</v>
       </c>
       <c r="F288">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G288">
         <v>0</v>
@@ -9397,7 +9644,7 @@
         <v>1</v>
       </c>
       <c r="F289">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G289">
         <v>0</v>
@@ -9643,7 +9890,7 @@
       <c r="C300" t="s">
         <v>649</v>
       </c>
-      <c r="D300" s="12" t="s">
+      <c r="D300" s="11" t="s">
         <v>648</v>
       </c>
       <c r="E300">
@@ -10106,8 +10353,17 @@
       <c r="D320" s="6" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E320">
+        <v>0</v>
+      </c>
+      <c r="F320">
+        <v>0</v>
+      </c>
+      <c r="G320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>81</v>
       </c>
@@ -10120,8 +10376,17 @@
       <c r="D321" s="6" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E321">
+        <v>0</v>
+      </c>
+      <c r="F321">
+        <v>0</v>
+      </c>
+      <c r="G321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>81</v>
       </c>
@@ -10134,8 +10399,17 @@
       <c r="D322" s="6" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E322">
+        <v>0</v>
+      </c>
+      <c r="F322">
+        <v>0</v>
+      </c>
+      <c r="G322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>81</v>
       </c>
@@ -10148,8 +10422,17 @@
       <c r="D323" s="6" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E323">
+        <v>0</v>
+      </c>
+      <c r="F323">
+        <v>0</v>
+      </c>
+      <c r="G323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>81</v>
       </c>
@@ -10162,8 +10445,17 @@
       <c r="D324" s="6" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E324">
+        <v>0</v>
+      </c>
+      <c r="F324">
+        <v>0</v>
+      </c>
+      <c r="G324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>81</v>
       </c>
@@ -10176,8 +10468,17 @@
       <c r="D325" s="6" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E325">
+        <v>0</v>
+      </c>
+      <c r="F325">
+        <v>0</v>
+      </c>
+      <c r="G325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>81</v>
       </c>
@@ -10190,8 +10491,17 @@
       <c r="D326" s="6" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E326">
+        <v>0</v>
+      </c>
+      <c r="F326">
+        <v>0</v>
+      </c>
+      <c r="G326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>81</v>
       </c>
@@ -10204,8 +10514,17 @@
       <c r="D327" s="6" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E327">
+        <v>0</v>
+      </c>
+      <c r="F327">
+        <v>0</v>
+      </c>
+      <c r="G327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>81</v>
       </c>
@@ -10218,8 +10537,17 @@
       <c r="D328" s="6" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E328">
+        <v>0</v>
+      </c>
+      <c r="F328">
+        <v>0</v>
+      </c>
+      <c r="G328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>82</v>
       </c>
@@ -10232,8 +10560,17 @@
       <c r="D329" s="6" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E329">
+        <v>0</v>
+      </c>
+      <c r="F329">
+        <v>0</v>
+      </c>
+      <c r="G329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>82</v>
       </c>
@@ -10246,8 +10583,17 @@
       <c r="D330" s="6" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E330">
+        <v>0</v>
+      </c>
+      <c r="F330">
+        <v>0</v>
+      </c>
+      <c r="G330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>82</v>
       </c>
@@ -10260,8 +10606,17 @@
       <c r="D331" s="6" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E331">
+        <v>0</v>
+      </c>
+      <c r="F331">
+        <v>0</v>
+      </c>
+      <c r="G331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>82</v>
       </c>
@@ -10274,8 +10629,17 @@
       <c r="D332" s="6" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E332">
+        <v>0</v>
+      </c>
+      <c r="F332">
+        <v>0</v>
+      </c>
+      <c r="G332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>82</v>
       </c>
@@ -10288,8 +10652,17 @@
       <c r="D333" s="6" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E333">
+        <v>0</v>
+      </c>
+      <c r="F333">
+        <v>0</v>
+      </c>
+      <c r="G333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>82</v>
       </c>
@@ -10302,8 +10675,17 @@
       <c r="D334" s="6" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E334">
+        <v>0</v>
+      </c>
+      <c r="F334">
+        <v>0</v>
+      </c>
+      <c r="G334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>82</v>
       </c>
@@ -10316,8 +10698,17 @@
       <c r="D335" s="6" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E335">
+        <v>0</v>
+      </c>
+      <c r="F335">
+        <v>0</v>
+      </c>
+      <c r="G335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>82</v>
       </c>
@@ -10330,8 +10721,17 @@
       <c r="D336" s="6" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E336">
+        <v>0</v>
+      </c>
+      <c r="F336">
+        <v>0</v>
+      </c>
+      <c r="G336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>82</v>
       </c>
@@ -10344,8 +10744,17 @@
       <c r="D337" s="6" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E337">
+        <v>0</v>
+      </c>
+      <c r="F337">
+        <v>0</v>
+      </c>
+      <c r="G337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>83</v>
       </c>
@@ -10358,8 +10767,17 @@
       <c r="D338" s="6" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E338">
+        <v>0</v>
+      </c>
+      <c r="F338">
+        <v>0</v>
+      </c>
+      <c r="G338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>83</v>
       </c>
@@ -10372,8 +10790,17 @@
       <c r="D339" s="6" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E339">
+        <v>0</v>
+      </c>
+      <c r="F339">
+        <v>0</v>
+      </c>
+      <c r="G339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>83</v>
       </c>
@@ -10386,8 +10813,17 @@
       <c r="D340" s="6" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E340">
+        <v>0</v>
+      </c>
+      <c r="F340">
+        <v>0</v>
+      </c>
+      <c r="G340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>83</v>
       </c>
@@ -10400,8 +10836,17 @@
       <c r="D341" s="6" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E341">
+        <v>0</v>
+      </c>
+      <c r="F341">
+        <v>0</v>
+      </c>
+      <c r="G341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>83</v>
       </c>
@@ -10414,8 +10859,17 @@
       <c r="D342" s="6" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E342">
+        <v>0</v>
+      </c>
+      <c r="F342">
+        <v>0</v>
+      </c>
+      <c r="G342">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>83</v>
       </c>
@@ -10428,8 +10882,17 @@
       <c r="D343" s="6" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E343">
+        <v>0</v>
+      </c>
+      <c r="F343">
+        <v>0</v>
+      </c>
+      <c r="G343">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>83</v>
       </c>
@@ -10442,8 +10905,17 @@
       <c r="D344" s="6" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E344">
+        <v>0</v>
+      </c>
+      <c r="F344">
+        <v>0</v>
+      </c>
+      <c r="G344">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>83</v>
       </c>
@@ -10456,8 +10928,17 @@
       <c r="D345" s="6" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E345">
+        <v>0</v>
+      </c>
+      <c r="F345">
+        <v>0</v>
+      </c>
+      <c r="G345">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>83</v>
       </c>
@@ -10470,8 +10951,17 @@
       <c r="D346" s="6" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E346">
+        <v>0</v>
+      </c>
+      <c r="F346">
+        <v>0</v>
+      </c>
+      <c r="G346">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>84</v>
       </c>
@@ -10484,8 +10974,17 @@
       <c r="D347" s="6" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E347">
+        <v>0</v>
+      </c>
+      <c r="F347">
+        <v>0</v>
+      </c>
+      <c r="G347">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>84</v>
       </c>
@@ -10498,8 +10997,17 @@
       <c r="D348" s="6" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E348">
+        <v>0</v>
+      </c>
+      <c r="F348">
+        <v>0</v>
+      </c>
+      <c r="G348">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>84</v>
       </c>
@@ -10512,8 +11020,17 @@
       <c r="D349" s="6" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E349">
+        <v>0</v>
+      </c>
+      <c r="F349">
+        <v>0</v>
+      </c>
+      <c r="G349">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>84</v>
       </c>
@@ -10526,8 +11043,17 @@
       <c r="D350" s="6" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E350">
+        <v>0</v>
+      </c>
+      <c r="F350">
+        <v>0</v>
+      </c>
+      <c r="G350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>84</v>
       </c>
@@ -10540,8 +11066,17 @@
       <c r="D351" s="6" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E351">
+        <v>0</v>
+      </c>
+      <c r="F351">
+        <v>0</v>
+      </c>
+      <c r="G351">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>84</v>
       </c>
@@ -10554,8 +11089,17 @@
       <c r="D352" s="6" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E352">
+        <v>0</v>
+      </c>
+      <c r="F352">
+        <v>0</v>
+      </c>
+      <c r="G352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>84</v>
       </c>
@@ -10568,8 +11112,17 @@
       <c r="D353" s="6" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E353">
+        <v>0</v>
+      </c>
+      <c r="F353">
+        <v>0</v>
+      </c>
+      <c r="G353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>84</v>
       </c>
@@ -10582,8 +11135,17 @@
       <c r="D354" s="6" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E354">
+        <v>0</v>
+      </c>
+      <c r="F354">
+        <v>0</v>
+      </c>
+      <c r="G354">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>84</v>
       </c>
@@ -10596,966 +11158,2685 @@
       <c r="D355" s="6" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="356" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E355">
+        <v>0</v>
+      </c>
+      <c r="F355">
+        <v>0</v>
+      </c>
+      <c r="G355">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A356" s="4" t="s">
         <v>511</v>
       </c>
       <c r="B356" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="D356" s="11"/>
-    </row>
-    <row r="357" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C356" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D356" s="6" t="s">
+        <v>705</v>
+      </c>
+      <c r="E356" s="4">
+        <v>1</v>
+      </c>
+      <c r="F356" s="4">
+        <v>0</v>
+      </c>
+      <c r="G356" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A357" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B357" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C357" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D357" s="6" t="s">
+        <v>706</v>
+      </c>
+      <c r="E357" s="4">
+        <v>1</v>
+      </c>
+      <c r="F357" s="4">
+        <v>0</v>
+      </c>
+      <c r="G357" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A358" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B358" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C358" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D358" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="E358" s="4">
+        <v>1</v>
+      </c>
+      <c r="F358" s="4">
+        <v>0</v>
+      </c>
+      <c r="G358" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A359" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B359" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C359" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D359" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="E359" s="4">
+        <v>1</v>
+      </c>
+      <c r="F359" s="4">
+        <v>0</v>
+      </c>
+      <c r="G359" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A360" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B360" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C360" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D360" s="6" t="s">
+        <v>709</v>
+      </c>
+      <c r="E360" s="4">
+        <v>1</v>
+      </c>
+      <c r="F360" s="4">
+        <v>0</v>
+      </c>
+      <c r="G360" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A361" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B361" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C361" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D361" s="6" t="s">
+        <v>710</v>
+      </c>
+      <c r="E361" s="4">
+        <v>1</v>
+      </c>
+      <c r="F361" s="4">
+        <v>0</v>
+      </c>
+      <c r="G361" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A362" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B362" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C362" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D362" s="6" t="s">
+        <v>711</v>
+      </c>
+      <c r="E362" s="4">
+        <v>1</v>
+      </c>
+      <c r="F362" s="4">
+        <v>0</v>
+      </c>
+      <c r="G362" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A363" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B363" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C363" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D363" s="6" t="s">
+        <v>712</v>
+      </c>
+      <c r="E363" s="4">
+        <v>1</v>
+      </c>
+      <c r="F363" s="4">
+        <v>0</v>
+      </c>
+      <c r="G363" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A364" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B364" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C364" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D364" s="6" t="s">
+        <v>713</v>
+      </c>
+      <c r="E364" s="4">
+        <v>1</v>
+      </c>
+      <c r="F364" s="4">
+        <v>0</v>
+      </c>
+      <c r="G364" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A365" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B365" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C365" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D365" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="E365" s="4">
+        <v>1</v>
+      </c>
+      <c r="F365" s="4">
+        <v>0</v>
+      </c>
+      <c r="G365" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="366" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A366" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B366" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C366" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D366" s="6" t="s">
+        <v>715</v>
+      </c>
+      <c r="E366" s="4">
+        <v>1</v>
+      </c>
+      <c r="F366" s="4">
+        <v>0</v>
+      </c>
+      <c r="G366" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A367" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B367" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C367" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D367" s="6" t="s">
+        <v>716</v>
+      </c>
+      <c r="E367" s="4">
+        <v>1</v>
+      </c>
+      <c r="F367" s="4">
+        <v>0</v>
+      </c>
+      <c r="G367" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A368" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B368" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C368" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D368" s="6" t="s">
+        <v>717</v>
+      </c>
+      <c r="E368" s="4">
+        <v>1</v>
+      </c>
+      <c r="F368" s="4">
+        <v>0</v>
+      </c>
+      <c r="G368" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A369" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B369" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C369" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D369" s="6" t="s">
+        <v>718</v>
+      </c>
+      <c r="E369" s="4">
+        <v>1</v>
+      </c>
+      <c r="F369" s="4">
+        <v>0</v>
+      </c>
+      <c r="G369" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A370" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B370" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C370" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D370" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="E370" s="4">
+        <v>1</v>
+      </c>
+      <c r="F370" s="4">
+        <v>0</v>
+      </c>
+      <c r="G370" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A371" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B371" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C371" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D371" s="6" t="s">
+        <v>720</v>
+      </c>
+      <c r="E371" s="4">
+        <v>1</v>
+      </c>
+      <c r="F371" s="4">
+        <v>0</v>
+      </c>
+      <c r="G371" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A372" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B372" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C372" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D372" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="E372" s="4">
+        <v>1</v>
+      </c>
+      <c r="F372" s="4">
+        <v>0</v>
+      </c>
+      <c r="G372" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A373" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B373" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C373" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D373" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="E373" s="4">
+        <v>1</v>
+      </c>
+      <c r="F373" s="4">
+        <v>0</v>
+      </c>
+      <c r="G373" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="374" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A374" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B374" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C374" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D374" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="E374" s="4">
+        <v>1</v>
+      </c>
+      <c r="F374" s="4">
+        <v>0</v>
+      </c>
+      <c r="G374" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A375" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="B357" s="4" t="s">
+      <c r="B375" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="D357" s="11"/>
-    </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A358" t="s">
+      <c r="C375" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="D375" s="6" t="s">
+        <v>725</v>
+      </c>
+      <c r="E375" s="4">
+        <v>0</v>
+      </c>
+      <c r="F375" s="4">
+        <v>0</v>
+      </c>
+      <c r="G375" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A376" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="B376" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="C376" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="D376" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="E376" s="4">
+        <v>0</v>
+      </c>
+      <c r="F376" s="4">
+        <v>0</v>
+      </c>
+      <c r="G376" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A377" t="s">
         <v>85</v>
       </c>
-      <c r="B358" t="s">
+      <c r="B377" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A359" t="s">
+      <c r="C377" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D377" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E377" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F377" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G377" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A378" t="s">
         <v>86</v>
       </c>
-      <c r="B359" t="s">
+      <c r="B378" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A360" t="s">
+      <c r="C378" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D378" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E378" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F378" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G378" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A379" t="s">
         <v>517</v>
       </c>
-      <c r="B360" t="s">
+      <c r="B379" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A361" t="s">
+      <c r="C379" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D379" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E379" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F379" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G379" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A380" t="s">
         <v>519</v>
       </c>
-      <c r="B361" t="s">
+      <c r="B380" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A362" t="s">
+      <c r="C380" t="s">
+        <v>521</v>
+      </c>
+      <c r="D380" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="E380">
+        <v>0</v>
+      </c>
+      <c r="F380">
+        <v>0</v>
+      </c>
+      <c r="G380">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A381" t="s">
+        <v>519</v>
+      </c>
+      <c r="B381" t="s">
+        <v>521</v>
+      </c>
+      <c r="C381" t="s">
+        <v>521</v>
+      </c>
+      <c r="D381" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="E381">
+        <v>0</v>
+      </c>
+      <c r="F381">
+        <v>0</v>
+      </c>
+      <c r="G381">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A382" t="s">
+        <v>519</v>
+      </c>
+      <c r="B382" t="s">
+        <v>521</v>
+      </c>
+      <c r="C382" t="s">
+        <v>521</v>
+      </c>
+      <c r="D382" s="6" t="s">
+        <v>729</v>
+      </c>
+      <c r="E382">
+        <v>0</v>
+      </c>
+      <c r="F382">
+        <v>1</v>
+      </c>
+      <c r="G382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A383" t="s">
         <v>520</v>
       </c>
-      <c r="B362" t="s">
+      <c r="B383" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A363" t="s">
+      <c r="C383" t="s">
+        <v>522</v>
+      </c>
+      <c r="D383" s="6" t="s">
+        <v>730</v>
+      </c>
+      <c r="E383">
+        <v>0</v>
+      </c>
+      <c r="F383">
+        <v>0</v>
+      </c>
+      <c r="G383">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A384" t="s">
         <v>87</v>
       </c>
-      <c r="B363" t="s">
+      <c r="B384" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A364" t="s">
+      <c r="C384" t="s">
+        <v>731</v>
+      </c>
+      <c r="D384" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="E384">
+        <v>1</v>
+      </c>
+      <c r="F384">
+        <v>0</v>
+      </c>
+      <c r="G384">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A385" t="s">
+        <v>87</v>
+      </c>
+      <c r="B385" t="s">
+        <v>523</v>
+      </c>
+      <c r="C385" t="s">
+        <v>731</v>
+      </c>
+      <c r="D385" s="6" t="s">
+        <v>733</v>
+      </c>
+      <c r="E385">
+        <v>1</v>
+      </c>
+      <c r="F385">
+        <v>0</v>
+      </c>
+      <c r="G385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A386" t="s">
+        <v>87</v>
+      </c>
+      <c r="B386" t="s">
+        <v>523</v>
+      </c>
+      <c r="C386" t="s">
+        <v>731</v>
+      </c>
+      <c r="D386" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="E386">
+        <v>1</v>
+      </c>
+      <c r="F386">
+        <v>1</v>
+      </c>
+      <c r="G386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A387" t="s">
         <v>524</v>
       </c>
-      <c r="B364" s="5" t="s">
+      <c r="B387" s="5" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A365" t="s">
+      <c r="C387" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="D387" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="E387">
+        <v>1</v>
+      </c>
+      <c r="F387">
+        <v>0</v>
+      </c>
+      <c r="G387">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A388" t="s">
+        <v>524</v>
+      </c>
+      <c r="B388" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="C388" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="D388" s="6" t="s">
+        <v>733</v>
+      </c>
+      <c r="E388">
+        <v>1</v>
+      </c>
+      <c r="F388">
+        <v>0</v>
+      </c>
+      <c r="G388">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A389" t="s">
+        <v>524</v>
+      </c>
+      <c r="B389" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="C389" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="D389" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="E389">
+        <v>1</v>
+      </c>
+      <c r="F389">
+        <v>1</v>
+      </c>
+      <c r="G389">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A390" t="s">
         <v>88</v>
       </c>
-      <c r="B365" t="s">
+      <c r="B390" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A366" t="s">
+      <c r="C390" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="D390" s="6" t="s">
+        <v>735</v>
+      </c>
+      <c r="E390">
+        <v>1</v>
+      </c>
+      <c r="F390">
+        <v>0</v>
+      </c>
+      <c r="G390">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A391" t="s">
         <v>89</v>
       </c>
-      <c r="B366" s="5" t="s">
+      <c r="B391" s="5" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A367" t="s">
+      <c r="C391" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="D391" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="E391">
+        <v>0</v>
+      </c>
+      <c r="F391">
+        <v>0</v>
+      </c>
+      <c r="G391">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A392" t="s">
+        <v>89</v>
+      </c>
+      <c r="B392" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="C392" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="D392" s="6" t="s">
+        <v>738</v>
+      </c>
+      <c r="E392">
+        <v>0</v>
+      </c>
+      <c r="F392">
+        <v>1</v>
+      </c>
+      <c r="G392">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A393" t="s">
         <v>90</v>
       </c>
-      <c r="B367" s="5" t="s">
+      <c r="B393" s="5" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A368" t="s">
+      <c r="C393" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="D393" s="6" t="s">
+        <v>739</v>
+      </c>
+      <c r="E393">
+        <v>0</v>
+      </c>
+      <c r="F393">
+        <v>0</v>
+      </c>
+      <c r="G393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A394" t="s">
+        <v>90</v>
+      </c>
+      <c r="B394" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="C394" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="D394" s="6" t="s">
+        <v>740</v>
+      </c>
+      <c r="E394">
+        <v>0</v>
+      </c>
+      <c r="F394">
+        <v>1</v>
+      </c>
+      <c r="G394">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A395" t="s">
         <v>91</v>
       </c>
-      <c r="B368" s="5" t="s">
+      <c r="B395" s="5" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A369" t="s">
+      <c r="C395" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D395" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E395" t="s">
+        <v>187</v>
+      </c>
+      <c r="F395" t="s">
+        <v>187</v>
+      </c>
+      <c r="G395" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="396" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A396" t="s">
         <v>531</v>
       </c>
-      <c r="B369" s="5" t="s">
+      <c r="B396" s="5" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A370" t="s">
+      <c r="C396" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="D396" s="6" t="s">
+        <v>741</v>
+      </c>
+      <c r="E396">
+        <v>0</v>
+      </c>
+      <c r="F396">
+        <v>0</v>
+      </c>
+      <c r="G396">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A397" t="s">
+        <v>531</v>
+      </c>
+      <c r="B397" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="C397" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="D397" s="6" t="s">
+        <v>742</v>
+      </c>
+      <c r="E397">
+        <v>0</v>
+      </c>
+      <c r="F397">
+        <v>1</v>
+      </c>
+      <c r="G397">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A398" t="s">
         <v>92</v>
       </c>
-      <c r="B370" s="5" t="s">
+      <c r="B398" s="5" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A371" t="s">
+      <c r="C398" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D398" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E398" t="s">
+        <v>187</v>
+      </c>
+      <c r="F398" t="s">
+        <v>187</v>
+      </c>
+      <c r="G398" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="399" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A399" t="s">
         <v>93</v>
       </c>
-      <c r="B371" s="5" t="s">
+      <c r="B399" s="5" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A372" t="s">
+      <c r="C399" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D399" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E399" t="s">
+        <v>187</v>
+      </c>
+      <c r="F399" t="s">
+        <v>187</v>
+      </c>
+      <c r="G399" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="400" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A400" t="s">
         <v>94</v>
       </c>
-      <c r="B372" s="5" t="s">
+      <c r="B400" s="5" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A373" t="s">
+      <c r="C400" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D400" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E400" t="s">
+        <v>187</v>
+      </c>
+      <c r="F400" t="s">
+        <v>187</v>
+      </c>
+      <c r="G400" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="401" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A401" t="s">
         <v>536</v>
       </c>
-      <c r="B373" s="5" t="s">
+      <c r="B401" s="5" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A374" t="s">
+      <c r="C401" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="D401" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="E401">
+        <v>0</v>
+      </c>
+      <c r="F401">
+        <v>0</v>
+      </c>
+      <c r="G401">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A402" t="s">
+        <v>536</v>
+      </c>
+      <c r="B402" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="C402" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="D402" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="E402">
+        <v>0</v>
+      </c>
+      <c r="F402">
+        <v>1</v>
+      </c>
+      <c r="G402">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A403" t="s">
         <v>95</v>
       </c>
-      <c r="B374" t="s">
+      <c r="B403" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A375" t="s">
+      <c r="C403" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D403" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E403" t="s">
+        <v>187</v>
+      </c>
+      <c r="F403" t="s">
+        <v>187</v>
+      </c>
+      <c r="G403" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A404" t="s">
         <v>96</v>
       </c>
-      <c r="B375" t="s">
+      <c r="B404" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A376" t="s">
+      <c r="C404" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D404" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="E404">
+        <v>1</v>
+      </c>
+      <c r="F404">
+        <v>1</v>
+      </c>
+      <c r="G404">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A405" t="s">
         <v>97</v>
       </c>
-      <c r="B376" t="s">
+      <c r="B405" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A377" t="s">
+      <c r="C405" t="s">
+        <v>747</v>
+      </c>
+      <c r="D405" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="E405">
+        <v>1</v>
+      </c>
+      <c r="F405">
+        <v>0</v>
+      </c>
+      <c r="G405">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A406" t="s">
+        <v>97</v>
+      </c>
+      <c r="B406" t="s">
+        <v>542</v>
+      </c>
+      <c r="C406" t="s">
+        <v>747</v>
+      </c>
+      <c r="D406" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="E406">
+        <v>1</v>
+      </c>
+      <c r="F406">
+        <v>0</v>
+      </c>
+      <c r="G406">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A407" t="s">
+        <v>97</v>
+      </c>
+      <c r="B407" t="s">
+        <v>542</v>
+      </c>
+      <c r="C407" t="s">
+        <v>747</v>
+      </c>
+      <c r="D407" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="E407">
+        <v>1</v>
+      </c>
+      <c r="F407">
+        <v>0</v>
+      </c>
+      <c r="G407">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="408" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A408" t="s">
         <v>98</v>
       </c>
-      <c r="B377" t="s">
+      <c r="B408" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A378" t="s">
+      <c r="C408" t="s">
+        <v>187</v>
+      </c>
+      <c r="D408" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="E408">
+        <v>1</v>
+      </c>
+      <c r="F408">
+        <v>1</v>
+      </c>
+      <c r="G408">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A409" t="s">
         <v>99</v>
       </c>
-      <c r="B378" t="s">
+      <c r="B409" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A379" t="s">
+      <c r="C409" t="s">
+        <v>537</v>
+      </c>
+      <c r="D409" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="E409">
+        <v>0</v>
+      </c>
+      <c r="F409">
+        <v>0</v>
+      </c>
+      <c r="G409">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="410" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A410" t="s">
         <v>100</v>
       </c>
-      <c r="B379" t="s">
+      <c r="B410" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A380" t="s">
+      <c r="C410" t="s">
+        <v>538</v>
+      </c>
+      <c r="D410" s="6" t="s">
+        <v>752</v>
+      </c>
+      <c r="E410">
+        <v>0</v>
+      </c>
+      <c r="F410">
+        <v>0</v>
+      </c>
+      <c r="G410">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A411" t="s">
+        <v>100</v>
+      </c>
+      <c r="B411" t="s">
+        <v>538</v>
+      </c>
+      <c r="C411" t="s">
+        <v>538</v>
+      </c>
+      <c r="D411" s="6" t="s">
+        <v>753</v>
+      </c>
+      <c r="E411" s="4">
+        <v>0</v>
+      </c>
+      <c r="F411" s="4">
+        <v>0</v>
+      </c>
+      <c r="G411" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A412" t="s">
+        <v>100</v>
+      </c>
+      <c r="B412" t="s">
+        <v>538</v>
+      </c>
+      <c r="C412" t="s">
+        <v>538</v>
+      </c>
+      <c r="D412" s="6" t="s">
+        <v>754</v>
+      </c>
+      <c r="E412" s="4">
+        <v>0</v>
+      </c>
+      <c r="F412" s="4">
+        <v>1</v>
+      </c>
+      <c r="G412" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A413" t="s">
         <v>101</v>
       </c>
-      <c r="B380" t="s">
+      <c r="B413" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A381" t="s">
+      <c r="C413" t="s">
+        <v>539</v>
+      </c>
+      <c r="D413" s="6" t="s">
+        <v>755</v>
+      </c>
+      <c r="E413" s="4">
+        <v>0</v>
+      </c>
+      <c r="F413" s="4">
+        <v>0</v>
+      </c>
+      <c r="G413" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A414" t="s">
+        <v>101</v>
+      </c>
+      <c r="B414" t="s">
+        <v>539</v>
+      </c>
+      <c r="C414" t="s">
+        <v>539</v>
+      </c>
+      <c r="D414" s="6" t="s">
+        <v>756</v>
+      </c>
+      <c r="E414" s="4">
+        <v>0</v>
+      </c>
+      <c r="F414" s="4">
+        <v>0</v>
+      </c>
+      <c r="G414" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A415" t="s">
+        <v>101</v>
+      </c>
+      <c r="B415" t="s">
+        <v>539</v>
+      </c>
+      <c r="C415" t="s">
+        <v>539</v>
+      </c>
+      <c r="D415" s="6" t="s">
+        <v>757</v>
+      </c>
+      <c r="E415" s="4">
+        <v>0</v>
+      </c>
+      <c r="F415" s="4">
+        <v>0</v>
+      </c>
+      <c r="G415" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A416" t="s">
         <v>102</v>
       </c>
-      <c r="B381" t="s">
+      <c r="B416" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A382" t="s">
+      <c r="C416" t="s">
+        <v>540</v>
+      </c>
+      <c r="D416" s="6" t="s">
+        <v>758</v>
+      </c>
+      <c r="E416" s="4">
+        <v>0</v>
+      </c>
+      <c r="F416" s="4">
+        <v>0</v>
+      </c>
+      <c r="G416">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A417" t="s">
+        <v>102</v>
+      </c>
+      <c r="B417" t="s">
+        <v>540</v>
+      </c>
+      <c r="C417" t="s">
+        <v>540</v>
+      </c>
+      <c r="D417" s="6" t="s">
+        <v>759</v>
+      </c>
+      <c r="E417" s="4">
+        <v>0</v>
+      </c>
+      <c r="F417" s="4">
+        <v>1</v>
+      </c>
+      <c r="G417">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A418" t="s">
         <v>103</v>
       </c>
-      <c r="B382" t="s">
+      <c r="B418" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A383" t="s">
+      <c r="C418" t="s">
+        <v>541</v>
+      </c>
+      <c r="D418" s="6" t="s">
+        <v>760</v>
+      </c>
+      <c r="E418" s="4">
+        <v>0</v>
+      </c>
+      <c r="F418" s="4">
+        <v>0</v>
+      </c>
+      <c r="G418">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A419" t="s">
         <v>104</v>
       </c>
-      <c r="B383" t="s">
+      <c r="B419" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A384" t="s">
+      <c r="C419" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D419" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E419" t="s">
+        <v>187</v>
+      </c>
+      <c r="F419" t="s">
+        <v>187</v>
+      </c>
+      <c r="G419" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="420" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A420" t="s">
         <v>105</v>
       </c>
-      <c r="B384" t="s">
+      <c r="B420" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A385" t="s">
+      <c r="C420" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D420" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E420" t="s">
+        <v>187</v>
+      </c>
+      <c r="F420" t="s">
+        <v>187</v>
+      </c>
+      <c r="G420" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="421" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A421" t="s">
         <v>106</v>
       </c>
-      <c r="B385" t="s">
+      <c r="B421" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A386" t="s">
+      <c r="C421" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D421" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E421" t="s">
+        <v>187</v>
+      </c>
+      <c r="F421" t="s">
+        <v>187</v>
+      </c>
+      <c r="G421" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="422" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A422" t="s">
         <v>107</v>
       </c>
-      <c r="B386" t="s">
+      <c r="B422" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A387" t="s">
+      <c r="C422" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D422" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E422" t="s">
+        <v>187</v>
+      </c>
+      <c r="F422" t="s">
+        <v>187</v>
+      </c>
+      <c r="G422" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="423" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A423" t="s">
         <v>108</v>
       </c>
-      <c r="B387" t="s">
+      <c r="B423" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A388" t="s">
+      <c r="C423" t="s">
+        <v>551</v>
+      </c>
+      <c r="D423" s="6" t="s">
+        <v>761</v>
+      </c>
+      <c r="E423">
+        <v>0</v>
+      </c>
+      <c r="F423">
+        <v>0</v>
+      </c>
+      <c r="G423">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="424" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A424" t="s">
+        <v>108</v>
+      </c>
+      <c r="B424" t="s">
+        <v>551</v>
+      </c>
+      <c r="C424" t="s">
+        <v>551</v>
+      </c>
+      <c r="D424" s="6" t="s">
+        <v>762</v>
+      </c>
+      <c r="E424">
+        <v>0</v>
+      </c>
+      <c r="F424">
+        <v>0</v>
+      </c>
+      <c r="G424">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A425" t="s">
+        <v>108</v>
+      </c>
+      <c r="B425" t="s">
+        <v>551</v>
+      </c>
+      <c r="C425" t="s">
+        <v>551</v>
+      </c>
+      <c r="D425" s="6" t="s">
+        <v>763</v>
+      </c>
+      <c r="E425">
+        <v>0</v>
+      </c>
+      <c r="F425">
+        <v>1</v>
+      </c>
+      <c r="G425">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A426" t="s">
         <v>109</v>
       </c>
-      <c r="B388" t="s">
+      <c r="B426" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A389" t="s">
+      <c r="C426" t="s">
+        <v>552</v>
+      </c>
+      <c r="D426" s="6" t="s">
+        <v>764</v>
+      </c>
+      <c r="E426">
+        <v>0</v>
+      </c>
+      <c r="F426">
+        <v>0</v>
+      </c>
+      <c r="G426">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A427" t="s">
+        <v>109</v>
+      </c>
+      <c r="B427" t="s">
+        <v>552</v>
+      </c>
+      <c r="C427" t="s">
+        <v>552</v>
+      </c>
+      <c r="D427" s="6" t="s">
+        <v>765</v>
+      </c>
+      <c r="E427">
+        <v>0</v>
+      </c>
+      <c r="F427">
+        <v>0</v>
+      </c>
+      <c r="G427">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A428" t="s">
         <v>110</v>
       </c>
-      <c r="B389" t="s">
+      <c r="B428" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A390" t="s">
+      <c r="C428" t="s">
+        <v>553</v>
+      </c>
+      <c r="D428" s="6" t="s">
+        <v>766</v>
+      </c>
+      <c r="E428">
+        <v>0</v>
+      </c>
+      <c r="F428">
+        <v>0</v>
+      </c>
+      <c r="G428">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A429" t="s">
+        <v>110</v>
+      </c>
+      <c r="B429" t="s">
+        <v>553</v>
+      </c>
+      <c r="C429" t="s">
+        <v>553</v>
+      </c>
+      <c r="D429" s="6" t="s">
+        <v>767</v>
+      </c>
+      <c r="E429">
+        <v>0</v>
+      </c>
+      <c r="F429">
+        <v>1</v>
+      </c>
+      <c r="G429">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="430" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A430" t="s">
         <v>556</v>
       </c>
-      <c r="B390" t="s">
+      <c r="B430" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A391" t="s">
+      <c r="C430" t="s">
+        <v>557</v>
+      </c>
+      <c r="D430" s="6" t="s">
+        <v>768</v>
+      </c>
+      <c r="E430">
+        <v>0</v>
+      </c>
+      <c r="F430">
+        <v>0</v>
+      </c>
+      <c r="G430">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A431" t="s">
+        <v>556</v>
+      </c>
+      <c r="B431" t="s">
+        <v>557</v>
+      </c>
+      <c r="C431" t="s">
+        <v>557</v>
+      </c>
+      <c r="D431" s="6" t="s">
+        <v>769</v>
+      </c>
+      <c r="E431">
+        <v>0</v>
+      </c>
+      <c r="F431">
+        <v>0</v>
+      </c>
+      <c r="G431">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A432" t="s">
+        <v>556</v>
+      </c>
+      <c r="B432" t="s">
+        <v>557</v>
+      </c>
+      <c r="C432" t="s">
+        <v>557</v>
+      </c>
+      <c r="D432" s="6" t="s">
+        <v>770</v>
+      </c>
+      <c r="E432">
+        <v>0</v>
+      </c>
+      <c r="F432">
+        <v>0</v>
+      </c>
+      <c r="G432">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A433" t="s">
+        <v>556</v>
+      </c>
+      <c r="B433" t="s">
+        <v>557</v>
+      </c>
+      <c r="C433" t="s">
+        <v>557</v>
+      </c>
+      <c r="D433" s="6" t="s">
+        <v>771</v>
+      </c>
+      <c r="E433">
+        <v>1</v>
+      </c>
+      <c r="F433">
+        <v>1</v>
+      </c>
+      <c r="G433">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A434" t="s">
         <v>111</v>
       </c>
-      <c r="B391" t="s">
+      <c r="B434" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A392" t="s">
+      <c r="C434" t="s">
+        <v>187</v>
+      </c>
+      <c r="D434" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E434" t="s">
+        <v>187</v>
+      </c>
+      <c r="F434" t="s">
+        <v>187</v>
+      </c>
+      <c r="G434" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="435" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A435" t="s">
         <v>558</v>
       </c>
-      <c r="B392" t="s">
+      <c r="B435" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A393" t="s">
+      <c r="C435" t="s">
+        <v>559</v>
+      </c>
+      <c r="D435" s="6" t="s">
+        <v>772</v>
+      </c>
+      <c r="E435">
+        <v>0</v>
+      </c>
+      <c r="F435">
+        <v>0</v>
+      </c>
+      <c r="G435">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="436" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A436" t="s">
+        <v>558</v>
+      </c>
+      <c r="B436" t="s">
+        <v>559</v>
+      </c>
+      <c r="C436" t="s">
+        <v>559</v>
+      </c>
+      <c r="D436" s="6" t="s">
+        <v>773</v>
+      </c>
+      <c r="E436">
+        <v>0</v>
+      </c>
+      <c r="F436">
+        <v>0</v>
+      </c>
+      <c r="G436">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="437" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A437" t="s">
+        <v>558</v>
+      </c>
+      <c r="B437" t="s">
+        <v>559</v>
+      </c>
+      <c r="C437" t="s">
+        <v>559</v>
+      </c>
+      <c r="D437" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="E437">
+        <v>0</v>
+      </c>
+      <c r="F437">
+        <v>0</v>
+      </c>
+      <c r="G437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A438" t="s">
+        <v>558</v>
+      </c>
+      <c r="B438" t="s">
+        <v>559</v>
+      </c>
+      <c r="C438" t="s">
+        <v>559</v>
+      </c>
+      <c r="D438" s="6" t="s">
+        <v>771</v>
+      </c>
+      <c r="E438">
+        <v>1</v>
+      </c>
+      <c r="F438">
+        <v>1</v>
+      </c>
+      <c r="G438">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A439" t="s">
         <v>112</v>
       </c>
-      <c r="B393" t="s">
+      <c r="B439" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A394" t="s">
+      <c r="C439" t="s">
+        <v>555</v>
+      </c>
+      <c r="D439" s="6" t="s">
+        <v>775</v>
+      </c>
+      <c r="E439">
+        <v>0</v>
+      </c>
+      <c r="F439">
+        <v>0</v>
+      </c>
+      <c r="G439">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A440" t="s">
+        <v>112</v>
+      </c>
+      <c r="B440" t="s">
+        <v>555</v>
+      </c>
+      <c r="C440" t="s">
+        <v>555</v>
+      </c>
+      <c r="D440" s="6" t="s">
+        <v>776</v>
+      </c>
+      <c r="E440">
+        <v>0</v>
+      </c>
+      <c r="F440">
+        <v>0</v>
+      </c>
+      <c r="G440">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A441" t="s">
         <v>560</v>
       </c>
-      <c r="B394" t="s">
+      <c r="B441" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A395" t="s">
+      <c r="C441" t="s">
+        <v>777</v>
+      </c>
+      <c r="D441" s="6" t="s">
+        <v>778</v>
+      </c>
+      <c r="E441">
+        <v>0</v>
+      </c>
+      <c r="F441">
+        <v>0</v>
+      </c>
+      <c r="G441">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A442" t="s">
+        <v>560</v>
+      </c>
+      <c r="B442" t="s">
+        <v>561</v>
+      </c>
+      <c r="C442" t="s">
+        <v>777</v>
+      </c>
+      <c r="D442" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="E442">
+        <v>0</v>
+      </c>
+      <c r="F442">
+        <v>0</v>
+      </c>
+      <c r="G442">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="443" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A443" t="s">
+        <v>560</v>
+      </c>
+      <c r="B443" t="s">
+        <v>561</v>
+      </c>
+      <c r="C443" t="s">
+        <v>777</v>
+      </c>
+      <c r="D443" s="6" t="s">
+        <v>780</v>
+      </c>
+      <c r="E443">
+        <v>1</v>
+      </c>
+      <c r="F443">
+        <v>1</v>
+      </c>
+      <c r="G443">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A444" t="s">
         <v>113</v>
       </c>
-      <c r="B395" t="s">
+      <c r="B444" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A396" t="s">
+    <row r="445" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A445" t="s">
         <v>114</v>
       </c>
-      <c r="B396" t="s">
+      <c r="B445" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A397" t="s">
+    <row r="446" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A446" t="s">
         <v>115</v>
       </c>
-      <c r="B397" t="s">
+      <c r="B446" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A398" t="s">
+    <row r="447" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A447" t="s">
         <v>116</v>
       </c>
-      <c r="B398" t="s">
+      <c r="B447" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A399" t="s">
+    <row r="448" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A448" t="s">
         <v>117</v>
       </c>
-      <c r="B399" t="s">
+      <c r="B448" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A400" t="s">
+    <row r="449" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A449" t="s">
         <v>570</v>
       </c>
-      <c r="B400" t="s">
+      <c r="B449" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A401" t="s">
+    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A450" t="s">
         <v>572</v>
       </c>
-      <c r="B401" t="s">
+      <c r="B450" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A402" t="s">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A451" t="s">
         <v>118</v>
       </c>
-      <c r="B402" t="s">
+      <c r="B451" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A403" t="s">
+    <row r="452" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A452" t="s">
         <v>119</v>
       </c>
-      <c r="B403" t="s">
+      <c r="B452" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A404" t="s">
+    <row r="453" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A453" t="s">
         <v>120</v>
       </c>
-      <c r="B404" t="s">
+      <c r="B453" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A405" t="s">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A454" t="s">
         <v>121</v>
       </c>
-      <c r="B405" t="s">
+      <c r="B454" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A406" t="s">
+    <row r="455" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A455" t="s">
         <v>579</v>
       </c>
-      <c r="B406" t="s">
+      <c r="B455" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A407" t="s">
+    <row r="456" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A456" t="s">
         <v>122</v>
       </c>
-      <c r="B407" t="s">
+      <c r="B456" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A408" t="s">
+    <row r="457" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A457" t="s">
         <v>123</v>
       </c>
-      <c r="B408" t="s">
+      <c r="B457" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A409" t="s">
+    <row r="458" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A458" t="s">
         <v>124</v>
       </c>
-      <c r="B409" t="s">
+      <c r="B458" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A410" t="s">
+    <row r="459" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A459" t="s">
         <v>125</v>
       </c>
-      <c r="B410" t="s">
+      <c r="B459" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A411" t="s">
+    <row r="460" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A460" t="s">
         <v>126</v>
       </c>
-      <c r="B411" t="s">
+      <c r="B460" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A412" t="s">
+    <row r="461" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A461" t="s">
         <v>127</v>
       </c>
-      <c r="B412" t="s">
+      <c r="B461" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A413" t="s">
+    <row r="462" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A462" t="s">
         <v>128</v>
       </c>
-      <c r="B413" t="s">
+      <c r="B462" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A414" t="s">
+    <row r="463" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A463" t="s">
         <v>129</v>
       </c>
-      <c r="B414" t="s">
+      <c r="B463" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A415" t="s">
+    <row r="464" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A464" t="s">
         <v>130</v>
       </c>
-      <c r="B415" t="s">
+      <c r="B464" t="s">
         <v>586</v>
-      </c>
-    </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A416" t="s">
-        <v>131</v>
-      </c>
-      <c r="B416" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A417" t="s">
-        <v>592</v>
-      </c>
-      <c r="B417" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A418" t="s">
-        <v>132</v>
-      </c>
-      <c r="B418" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A419" t="s">
-        <v>133</v>
-      </c>
-      <c r="B419" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A420" t="s">
-        <v>134</v>
-      </c>
-      <c r="B420" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A421" t="s">
-        <v>135</v>
-      </c>
-      <c r="B421" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A422" t="s">
-        <v>136</v>
-      </c>
-      <c r="B422" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A423" t="s">
-        <v>137</v>
-      </c>
-      <c r="B423" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A424" t="s">
-        <v>138</v>
-      </c>
-      <c r="B424" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A425" t="s">
-        <v>139</v>
-      </c>
-      <c r="B425" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A426" t="s">
-        <v>140</v>
-      </c>
-      <c r="B426" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A427" t="s">
-        <v>141</v>
-      </c>
-      <c r="B427" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A428" t="s">
-        <v>142</v>
-      </c>
-      <c r="B428" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A429" t="s">
-        <v>143</v>
-      </c>
-      <c r="B429" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A430" t="s">
-        <v>144</v>
-      </c>
-      <c r="B430" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A431" t="s">
-        <v>145</v>
-      </c>
-      <c r="B431" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A432" t="s">
-        <v>146</v>
-      </c>
-      <c r="B432" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A433" t="s">
-        <v>147</v>
-      </c>
-      <c r="B433" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A434" t="s">
-        <v>148</v>
-      </c>
-      <c r="B434" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A435" t="s">
-        <v>149</v>
-      </c>
-      <c r="B435" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A436" t="s">
-        <v>150</v>
-      </c>
-      <c r="B436" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A437" t="s">
-        <v>151</v>
-      </c>
-      <c r="B437" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A438" t="s">
-        <v>152</v>
-      </c>
-      <c r="B438" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A439" t="s">
-        <v>153</v>
-      </c>
-      <c r="B439" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A440" t="s">
-        <v>154</v>
-      </c>
-      <c r="B440" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A441" t="s">
-        <v>155</v>
-      </c>
-      <c r="B441" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A442" t="s">
-        <v>156</v>
-      </c>
-      <c r="B442" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A443" t="s">
-        <v>157</v>
-      </c>
-      <c r="B443" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A444" t="s">
-        <v>158</v>
-      </c>
-      <c r="B444" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A445" t="s">
-        <v>159</v>
-      </c>
-      <c r="B445" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A446" t="s">
-        <v>160</v>
-      </c>
-      <c r="B446" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A447" t="s">
-        <v>161</v>
-      </c>
-      <c r="B447" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A448" t="s">
-        <v>162</v>
-      </c>
-      <c r="B448" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="449" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A449" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="450" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A450" t="s">
-        <v>164</v>
-      </c>
-      <c r="B450" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="451" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A451" t="s">
-        <v>165</v>
-      </c>
-      <c r="B451" t="s">
-        <v>621</v>
-      </c>
-      <c r="C451" t="s">
-        <v>498</v>
-      </c>
-      <c r="D451" s="6" t="s">
-        <v>499</v>
-      </c>
-      <c r="E451">
-        <v>0</v>
-      </c>
-      <c r="F451">
-        <v>0</v>
-      </c>
-      <c r="G451">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="452" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A452" t="s">
-        <v>165</v>
-      </c>
-      <c r="B452" t="s">
-        <v>621</v>
-      </c>
-      <c r="C452" t="s">
-        <v>498</v>
-      </c>
-      <c r="D452" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E452">
-        <v>0</v>
-      </c>
-      <c r="F452">
-        <v>0</v>
-      </c>
-      <c r="G452">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="453" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A453" t="s">
-        <v>166</v>
-      </c>
-      <c r="B453" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="454" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A454" t="s">
-        <v>167</v>
-      </c>
-      <c r="B454" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="455" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A455" t="s">
-        <v>168</v>
-      </c>
-      <c r="B455" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="456" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A456" t="s">
-        <v>169</v>
-      </c>
-      <c r="B456" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="457" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A457" t="s">
-        <v>170</v>
-      </c>
-      <c r="B457" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="458" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A458" t="s">
-        <v>171</v>
-      </c>
-      <c r="B458" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="459" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A459" t="s">
-        <v>172</v>
-      </c>
-      <c r="B459" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="460" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A460" t="s">
-        <v>173</v>
-      </c>
-      <c r="B460" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="461" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A461" t="s">
-        <v>174</v>
-      </c>
-      <c r="B461" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="462" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A462" t="s">
-        <v>175</v>
-      </c>
-      <c r="B462" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="463" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A463" t="s">
-        <v>176</v>
-      </c>
-      <c r="B463" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="464" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A464" t="s">
-        <v>177</v>
-      </c>
-      <c r="B464" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
-        <v>178</v>
+        <v>131</v>
       </c>
       <c r="B465" t="s">
-        <v>631</v>
+        <v>587</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
-        <v>179</v>
+        <v>592</v>
       </c>
       <c r="B466" t="s">
-        <v>632</v>
+        <v>593</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
       <c r="B467" t="s">
-        <v>633</v>
+        <v>594</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
-        <v>181</v>
+        <v>133</v>
       </c>
       <c r="B468" t="s">
-        <v>634</v>
+        <v>596</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
-        <v>182</v>
+        <v>134</v>
       </c>
       <c r="B469" t="s">
-        <v>635</v>
+        <v>597</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
-        <v>183</v>
+        <v>135</v>
       </c>
       <c r="B470" t="s">
-        <v>636</v>
+        <v>598</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
-        <v>184</v>
+        <v>136</v>
       </c>
       <c r="B471" t="s">
-        <v>561</v>
+        <v>599</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
+        <v>137</v>
+      </c>
+      <c r="B472" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A473" t="s">
+        <v>138</v>
+      </c>
+      <c r="B473" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A474" t="s">
+        <v>139</v>
+      </c>
+      <c r="B474" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A475" t="s">
+        <v>140</v>
+      </c>
+      <c r="B475" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A476" t="s">
+        <v>141</v>
+      </c>
+      <c r="B476" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A477" t="s">
+        <v>142</v>
+      </c>
+      <c r="B477" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A478" t="s">
+        <v>143</v>
+      </c>
+      <c r="B478" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A479" t="s">
+        <v>144</v>
+      </c>
+      <c r="B479" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A480" t="s">
+        <v>145</v>
+      </c>
+      <c r="B480" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A481" t="s">
+        <v>146</v>
+      </c>
+      <c r="B481" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A482" t="s">
+        <v>147</v>
+      </c>
+      <c r="B482" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A483" t="s">
+        <v>148</v>
+      </c>
+      <c r="B483" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A484" t="s">
+        <v>149</v>
+      </c>
+      <c r="B484" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A485" t="s">
+        <v>150</v>
+      </c>
+      <c r="B485" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A486" t="s">
+        <v>151</v>
+      </c>
+      <c r="B486" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A487" t="s">
+        <v>152</v>
+      </c>
+      <c r="B487" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A488" t="s">
+        <v>153</v>
+      </c>
+      <c r="B488" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A489" t="s">
+        <v>154</v>
+      </c>
+      <c r="B489" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A490" t="s">
+        <v>155</v>
+      </c>
+      <c r="B490" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A491" t="s">
+        <v>156</v>
+      </c>
+      <c r="B491" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A492" t="s">
+        <v>157</v>
+      </c>
+      <c r="B492" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A493" t="s">
+        <v>158</v>
+      </c>
+      <c r="B493" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A494" t="s">
+        <v>159</v>
+      </c>
+      <c r="B494" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A495" t="s">
+        <v>160</v>
+      </c>
+      <c r="B495" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A496" t="s">
+        <v>161</v>
+      </c>
+      <c r="B496" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="497" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A497" t="s">
+        <v>162</v>
+      </c>
+      <c r="B497" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="498" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A498" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="499" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A499" t="s">
+        <v>164</v>
+      </c>
+      <c r="B499" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="500" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A500" t="s">
+        <v>165</v>
+      </c>
+      <c r="B500" t="s">
+        <v>621</v>
+      </c>
+      <c r="C500" t="s">
+        <v>498</v>
+      </c>
+      <c r="D500" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="E500">
+        <v>0</v>
+      </c>
+      <c r="F500">
+        <v>0</v>
+      </c>
+      <c r="G500">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="501" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A501" t="s">
+        <v>165</v>
+      </c>
+      <c r="B501" t="s">
+        <v>621</v>
+      </c>
+      <c r="C501" t="s">
+        <v>498</v>
+      </c>
+      <c r="D501" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E501">
+        <v>0</v>
+      </c>
+      <c r="F501">
+        <v>0</v>
+      </c>
+      <c r="G501">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="502" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A502" t="s">
+        <v>166</v>
+      </c>
+      <c r="B502" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="503" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A503" t="s">
+        <v>167</v>
+      </c>
+      <c r="B503" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="504" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A504" t="s">
+        <v>168</v>
+      </c>
+      <c r="B504" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="505" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A505" t="s">
+        <v>169</v>
+      </c>
+      <c r="B505" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="506" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A506" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B506" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="507" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A507" t="s">
+        <v>171</v>
+      </c>
+      <c r="B507" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="508" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A508" t="s">
+        <v>172</v>
+      </c>
+      <c r="B508" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="509" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A509" t="s">
+        <v>173</v>
+      </c>
+      <c r="B509" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="510" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A510" t="s">
+        <v>174</v>
+      </c>
+      <c r="B510" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="511" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A511" t="s">
+        <v>175</v>
+      </c>
+      <c r="B511" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="512" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A512" t="s">
+        <v>176</v>
+      </c>
+      <c r="B512" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="513" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A513" t="s">
+        <v>177</v>
+      </c>
+      <c r="B513" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="514" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A514" t="s">
+        <v>178</v>
+      </c>
+      <c r="B514" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="515" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A515" t="s">
+        <v>179</v>
+      </c>
+      <c r="B515" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="516" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A516" t="s">
+        <v>180</v>
+      </c>
+      <c r="B516" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="517" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A517" t="s">
+        <v>181</v>
+      </c>
+      <c r="B517" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="518" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A518" t="s">
+        <v>182</v>
+      </c>
+      <c r="B518" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="519" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A519" t="s">
+        <v>183</v>
+      </c>
+      <c r="B519" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="520" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A520" t="s">
+        <v>184</v>
+      </c>
+      <c r="B520" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="521" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A521" t="s">
         <v>185</v>
       </c>
     </row>

</xml_diff>

<commit_message>
arancel aduanero listo hasta picoroco
</commit_message>
<xml_diff>
--- a/information/raw_databases/ADUANAS_CHILE/arancel_aduanero_nomenclatura/arancel_aduanero_2017/codigos_aduana_por_especie_2017.xlsx
+++ b/information/raw_databases/ADUANAS_CHILE/arancel_aduanero_nomenclatura/arancel_aduanero_2017/codigos_aduana_por_especie_2017.xlsx
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2121" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2596" uniqueCount="861">
   <si>
     <t>especie_SERNAPESCA</t>
   </si>
@@ -2546,13 +2546,253 @@
   </si>
   <si>
     <t>1605.5100</t>
+  </si>
+  <si>
+    <t>0307.5110</t>
+  </si>
+  <si>
+    <t>Octopus mimus</t>
+  </si>
+  <si>
+    <t>0307.5210</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enteroctopus megalocyathus</t>
+  </si>
+  <si>
+    <t>0307.5120</t>
+  </si>
+  <si>
+    <t>0307.5220</t>
+  </si>
+  <si>
+    <t>0307.7214</t>
+  </si>
+  <si>
+    <t>0306.1711</t>
+  </si>
+  <si>
+    <t>0306.3611</t>
+  </si>
+  <si>
+    <t>1605.2111</t>
+  </si>
+  <si>
+    <t>1605.2121</t>
+  </si>
+  <si>
+    <t>1605.2911</t>
+  </si>
+  <si>
+    <t>0306.1713</t>
+  </si>
+  <si>
+    <t>0306.3613</t>
+  </si>
+  <si>
+    <t>1605.2113</t>
+  </si>
+  <si>
+    <t>1605.2123</t>
+  </si>
+  <si>
+    <t>1605.2913</t>
+  </si>
+  <si>
+    <t>0306.1712</t>
+  </si>
+  <si>
+    <t>0306.3612</t>
+  </si>
+  <si>
+    <t>1605.2112</t>
+  </si>
+  <si>
+    <t>1605.2122</t>
+  </si>
+  <si>
+    <t>1605.2912</t>
+  </si>
+  <si>
+    <t>0306.1421</t>
+  </si>
+  <si>
+    <t>0306.3321</t>
+  </si>
+  <si>
+    <t>1605.1022</t>
+  </si>
+  <si>
+    <t>1605.1026</t>
+  </si>
+  <si>
+    <t>0306.1423</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CENTOLLON DEL NORTE                      </t>
+  </si>
+  <si>
+    <t>Paralomis spp</t>
+  </si>
+  <si>
+    <t>0306.1424</t>
+  </si>
+  <si>
+    <t>0306.3323</t>
+  </si>
+  <si>
+    <t>0306.3324</t>
+  </si>
+  <si>
+    <t>1605.1023</t>
+  </si>
+  <si>
+    <t>1605.1024</t>
+  </si>
+  <si>
+    <t>1605.1028</t>
+  </si>
+  <si>
+    <t>1605.1029</t>
+  </si>
+  <si>
+    <t>0306.1791</t>
+  </si>
+  <si>
+    <t>0306.3691</t>
+  </si>
+  <si>
+    <t>1605.2151</t>
+  </si>
+  <si>
+    <t>1605.2161</t>
+  </si>
+  <si>
+    <t>1605.2931</t>
+  </si>
+  <si>
+    <t>0306.1410</t>
+  </si>
+  <si>
+    <t>0306.3310</t>
+  </si>
+  <si>
+    <t>1605.1011</t>
+  </si>
+  <si>
+    <t>1605.1012</t>
+  </si>
+  <si>
+    <t>1605.1019</t>
+  </si>
+  <si>
+    <t>0306.1110</t>
+  </si>
+  <si>
+    <t>0306.3110</t>
+  </si>
+  <si>
+    <t>0306.3120</t>
+  </si>
+  <si>
+    <t>0306.1120</t>
+  </si>
+  <si>
+    <t>0306.1721</t>
+  </si>
+  <si>
+    <t>0306.3621</t>
+  </si>
+  <si>
+    <t>1605.2131</t>
+  </si>
+  <si>
+    <t>1605.2141</t>
+  </si>
+  <si>
+    <t>0306.1722</t>
+  </si>
+  <si>
+    <t>0306.3622</t>
+  </si>
+  <si>
+    <t>1605.2132</t>
+  </si>
+  <si>
+    <t>1605.2142</t>
+  </si>
+  <si>
+    <t>0302.3400</t>
+  </si>
+  <si>
+    <t>0303.4400</t>
+  </si>
+  <si>
+    <t>0304.4920</t>
+  </si>
+  <si>
+    <t>0304.8920</t>
+  </si>
+  <si>
+    <t>0305.3960</t>
+  </si>
+  <si>
+    <t>0303.8961</t>
+  </si>
+  <si>
+    <t>0303.8962</t>
+  </si>
+  <si>
+    <t>0303.8969</t>
+  </si>
+  <si>
+    <t>0302.8141</t>
+  </si>
+  <si>
+    <t>0302.9241</t>
+  </si>
+  <si>
+    <t>0303.8141</t>
+  </si>
+  <si>
+    <t>0303.9241</t>
+  </si>
+  <si>
+    <t>0304.4741</t>
+  </si>
+  <si>
+    <t>0304.5641</t>
+  </si>
+  <si>
+    <t>0304.8841</t>
+  </si>
+  <si>
+    <t>0304.9641</t>
+  </si>
+  <si>
+    <t>0305.7141</t>
+  </si>
+  <si>
+    <t>0307.5190</t>
+  </si>
+  <si>
+    <t>Octopus spp</t>
+  </si>
+  <si>
+    <t>0307.5290</t>
+  </si>
+  <si>
+    <t>0306.1130</t>
+  </si>
+  <si>
+    <t>0306.3130</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2613,6 +2853,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2637,7 +2884,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2647,8 +2894,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -2664,16 +2913,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2986,11 +3238,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G521"/>
+  <dimension ref="A1:G609"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A494" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D445" sqref="D445"/>
+      <pane ySplit="1" topLeftCell="A551" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H573" sqref="H573"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13199,462 +13451,1305 @@
       <c r="B444" t="s">
         <v>563</v>
       </c>
+      <c r="C444" t="s">
+        <v>782</v>
+      </c>
+      <c r="D444" s="6" t="s">
+        <v>781</v>
+      </c>
+      <c r="E444">
+        <v>0</v>
+      </c>
+      <c r="F444">
+        <v>0</v>
+      </c>
+      <c r="G444">
+        <v>1</v>
+      </c>
     </row>
     <row r="445" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B445" t="s">
-        <v>564</v>
+        <v>563</v>
+      </c>
+      <c r="C445" t="s">
+        <v>782</v>
+      </c>
+      <c r="D445" s="6" t="s">
+        <v>783</v>
+      </c>
+      <c r="E445">
+        <v>0</v>
+      </c>
+      <c r="F445">
+        <v>0</v>
+      </c>
+      <c r="G445">
+        <v>0</v>
       </c>
     </row>
     <row r="446" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B446" t="s">
-        <v>565</v>
+        <v>564</v>
+      </c>
+      <c r="C446" s="8" t="s">
+        <v>784</v>
+      </c>
+      <c r="D446" s="6" t="s">
+        <v>785</v>
+      </c>
+      <c r="E446">
+        <v>0</v>
+      </c>
+      <c r="F446">
+        <v>0</v>
+      </c>
+      <c r="G446">
+        <v>1</v>
       </c>
     </row>
     <row r="447" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B447" t="s">
-        <v>566</v>
+        <v>564</v>
+      </c>
+      <c r="C447" s="8" t="s">
+        <v>784</v>
+      </c>
+      <c r="D447" s="6" t="s">
+        <v>786</v>
+      </c>
+      <c r="E447">
+        <v>0</v>
+      </c>
+      <c r="F447">
+        <v>0</v>
+      </c>
+      <c r="G447">
+        <v>0</v>
       </c>
     </row>
     <row r="448" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
+        <v>115</v>
+      </c>
+      <c r="B448" t="s">
+        <v>565</v>
+      </c>
+      <c r="C448" t="s">
+        <v>187</v>
+      </c>
+      <c r="D448" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E448" t="s">
+        <v>187</v>
+      </c>
+      <c r="F448" t="s">
+        <v>187</v>
+      </c>
+      <c r="G448" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="449" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A449" t="s">
+        <v>116</v>
+      </c>
+      <c r="B449" t="s">
+        <v>566</v>
+      </c>
+      <c r="C449" t="s">
+        <v>566</v>
+      </c>
+      <c r="D449" s="6" t="s">
+        <v>787</v>
+      </c>
+      <c r="E449">
+        <v>0</v>
+      </c>
+      <c r="F449">
+        <v>0</v>
+      </c>
+      <c r="G449">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A450" t="s">
         <v>117</v>
       </c>
-      <c r="B448" t="s">
+      <c r="B450" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A449" t="s">
+      <c r="C450" t="s">
+        <v>567</v>
+      </c>
+      <c r="D450" s="6" t="s">
+        <v>788</v>
+      </c>
+      <c r="E450">
+        <v>0</v>
+      </c>
+      <c r="F450">
+        <v>0</v>
+      </c>
+      <c r="G450">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A451" t="s">
+        <v>117</v>
+      </c>
+      <c r="B451" t="s">
+        <v>567</v>
+      </c>
+      <c r="C451" t="s">
+        <v>567</v>
+      </c>
+      <c r="D451" s="6" t="s">
+        <v>789</v>
+      </c>
+      <c r="E451">
+        <v>0</v>
+      </c>
+      <c r="F451">
+        <v>0</v>
+      </c>
+      <c r="G451">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A452" t="s">
+        <v>117</v>
+      </c>
+      <c r="B452" t="s">
+        <v>567</v>
+      </c>
+      <c r="C452" t="s">
+        <v>567</v>
+      </c>
+      <c r="D452" s="6" t="s">
+        <v>790</v>
+      </c>
+      <c r="E452">
+        <v>0</v>
+      </c>
+      <c r="F452">
+        <v>1</v>
+      </c>
+      <c r="G452">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A453" t="s">
+        <v>117</v>
+      </c>
+      <c r="B453" t="s">
+        <v>567</v>
+      </c>
+      <c r="C453" t="s">
+        <v>567</v>
+      </c>
+      <c r="D453" s="6" t="s">
+        <v>791</v>
+      </c>
+      <c r="E453">
+        <v>0</v>
+      </c>
+      <c r="F453">
+        <v>1</v>
+      </c>
+      <c r="G453">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="454" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A454" t="s">
+        <v>117</v>
+      </c>
+      <c r="B454" t="s">
+        <v>567</v>
+      </c>
+      <c r="C454" t="s">
+        <v>567</v>
+      </c>
+      <c r="D454" s="6" t="s">
+        <v>792</v>
+      </c>
+      <c r="E454">
+        <v>0</v>
+      </c>
+      <c r="F454">
+        <v>1</v>
+      </c>
+      <c r="G454">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A455" t="s">
         <v>570</v>
       </c>
-      <c r="B449" t="s">
+      <c r="B455" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A450" t="s">
+      <c r="C455" t="s">
+        <v>571</v>
+      </c>
+      <c r="D455" s="6" t="s">
+        <v>793</v>
+      </c>
+      <c r="E455">
+        <v>0</v>
+      </c>
+      <c r="F455">
+        <v>0</v>
+      </c>
+      <c r="G455">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A456" t="s">
+        <v>570</v>
+      </c>
+      <c r="B456" t="s">
+        <v>571</v>
+      </c>
+      <c r="C456" t="s">
+        <v>571</v>
+      </c>
+      <c r="D456" s="6" t="s">
+        <v>794</v>
+      </c>
+      <c r="E456">
+        <v>0</v>
+      </c>
+      <c r="F456">
+        <v>0</v>
+      </c>
+      <c r="G456">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A457" t="s">
+        <v>570</v>
+      </c>
+      <c r="B457" t="s">
+        <v>571</v>
+      </c>
+      <c r="C457" t="s">
+        <v>571</v>
+      </c>
+      <c r="D457" s="6" t="s">
+        <v>795</v>
+      </c>
+      <c r="E457">
+        <v>0</v>
+      </c>
+      <c r="F457">
+        <v>1</v>
+      </c>
+      <c r="G457">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A458" t="s">
+        <v>570</v>
+      </c>
+      <c r="B458" t="s">
+        <v>571</v>
+      </c>
+      <c r="C458" t="s">
+        <v>571</v>
+      </c>
+      <c r="D458" s="6" t="s">
+        <v>796</v>
+      </c>
+      <c r="E458">
+        <v>0</v>
+      </c>
+      <c r="F458">
+        <v>1</v>
+      </c>
+      <c r="G458">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="459" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A459" t="s">
+        <v>570</v>
+      </c>
+      <c r="B459" t="s">
+        <v>571</v>
+      </c>
+      <c r="C459" t="s">
+        <v>571</v>
+      </c>
+      <c r="D459" s="6" t="s">
+        <v>797</v>
+      </c>
+      <c r="E459">
+        <v>0</v>
+      </c>
+      <c r="F459">
+        <v>1</v>
+      </c>
+      <c r="G459">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="460" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A460" t="s">
         <v>572</v>
       </c>
-      <c r="B450" t="s">
+      <c r="B460" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A451" t="s">
+      <c r="C460" t="s">
+        <v>573</v>
+      </c>
+      <c r="D460" s="6" t="s">
+        <v>798</v>
+      </c>
+      <c r="E460">
+        <v>0</v>
+      </c>
+      <c r="F460">
+        <v>0</v>
+      </c>
+      <c r="G460">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="461" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A461" t="s">
+        <v>572</v>
+      </c>
+      <c r="B461" t="s">
+        <v>573</v>
+      </c>
+      <c r="C461" t="s">
+        <v>573</v>
+      </c>
+      <c r="D461" s="6" t="s">
+        <v>799</v>
+      </c>
+      <c r="E461">
+        <v>0</v>
+      </c>
+      <c r="F461">
+        <v>0</v>
+      </c>
+      <c r="G461">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="462" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A462" t="s">
+        <v>572</v>
+      </c>
+      <c r="B462" t="s">
+        <v>573</v>
+      </c>
+      <c r="C462" t="s">
+        <v>573</v>
+      </c>
+      <c r="D462" s="6" t="s">
+        <v>800</v>
+      </c>
+      <c r="E462">
+        <v>0</v>
+      </c>
+      <c r="F462">
+        <v>1</v>
+      </c>
+      <c r="G462">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="463" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A463" t="s">
+        <v>572</v>
+      </c>
+      <c r="B463" t="s">
+        <v>573</v>
+      </c>
+      <c r="C463" t="s">
+        <v>573</v>
+      </c>
+      <c r="D463" s="6" t="s">
+        <v>801</v>
+      </c>
+      <c r="E463">
+        <v>0</v>
+      </c>
+      <c r="F463">
+        <v>1</v>
+      </c>
+      <c r="G463">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="464" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A464" t="s">
+        <v>572</v>
+      </c>
+      <c r="B464" t="s">
+        <v>573</v>
+      </c>
+      <c r="C464" t="s">
+        <v>573</v>
+      </c>
+      <c r="D464" s="6" t="s">
+        <v>802</v>
+      </c>
+      <c r="E464">
+        <v>0</v>
+      </c>
+      <c r="F464">
+        <v>1</v>
+      </c>
+      <c r="G464">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A465" t="s">
         <v>118</v>
       </c>
-      <c r="B451" t="s">
+      <c r="B465" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="452" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A452" t="s">
+      <c r="C465" t="s">
+        <v>187</v>
+      </c>
+      <c r="D465" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E465" t="s">
+        <v>187</v>
+      </c>
+      <c r="F465" t="s">
+        <v>187</v>
+      </c>
+      <c r="G465" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="466" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A466" t="s">
         <v>119</v>
       </c>
-      <c r="B452" t="s">
+      <c r="B466" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="453" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A453" t="s">
+      <c r="C466" t="s">
+        <v>575</v>
+      </c>
+      <c r="D466" s="6" t="s">
+        <v>803</v>
+      </c>
+      <c r="E466">
+        <v>0</v>
+      </c>
+      <c r="F466">
+        <v>0</v>
+      </c>
+      <c r="G466">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A467" t="s">
+        <v>119</v>
+      </c>
+      <c r="B467" t="s">
+        <v>575</v>
+      </c>
+      <c r="C467" t="s">
+        <v>575</v>
+      </c>
+      <c r="D467" s="6" t="s">
+        <v>804</v>
+      </c>
+      <c r="E467">
+        <v>0</v>
+      </c>
+      <c r="F467">
+        <v>0</v>
+      </c>
+      <c r="G467">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="468" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A468" t="s">
+        <v>119</v>
+      </c>
+      <c r="B468" t="s">
+        <v>575</v>
+      </c>
+      <c r="C468" t="s">
+        <v>575</v>
+      </c>
+      <c r="D468" s="6" t="s">
+        <v>805</v>
+      </c>
+      <c r="E468">
+        <v>0</v>
+      </c>
+      <c r="F468">
+        <v>1</v>
+      </c>
+      <c r="G468">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="469" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A469" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B469" s="13" t="s">
+        <v>575</v>
+      </c>
+      <c r="C469" s="13" t="s">
+        <v>575</v>
+      </c>
+      <c r="D469" s="6" t="s">
+        <v>806</v>
+      </c>
+      <c r="E469">
+        <v>0</v>
+      </c>
+      <c r="F469">
+        <v>1</v>
+      </c>
+      <c r="G469">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="470" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A470" t="s">
         <v>120</v>
       </c>
-      <c r="B453" t="s">
+      <c r="B470" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="454" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A454" t="s">
+      <c r="C470" t="s">
+        <v>577</v>
+      </c>
+      <c r="D470" s="6" t="s">
+        <v>807</v>
+      </c>
+      <c r="E470">
+        <v>0</v>
+      </c>
+      <c r="F470">
+        <v>0</v>
+      </c>
+      <c r="G470">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="471" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A471" t="s">
+        <v>808</v>
+      </c>
+      <c r="B471" t="s">
+        <v>187</v>
+      </c>
+      <c r="C471" t="s">
+        <v>809</v>
+      </c>
+      <c r="D471" s="6" t="s">
+        <v>810</v>
+      </c>
+      <c r="E471">
+        <v>0</v>
+      </c>
+      <c r="F471">
+        <v>0</v>
+      </c>
+      <c r="G471">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="472" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A472" t="s">
+        <v>120</v>
+      </c>
+      <c r="B472" t="s">
+        <v>577</v>
+      </c>
+      <c r="C472" t="s">
+        <v>577</v>
+      </c>
+      <c r="D472" s="6" t="s">
+        <v>811</v>
+      </c>
+      <c r="E472">
+        <v>0</v>
+      </c>
+      <c r="F472">
+        <v>0</v>
+      </c>
+      <c r="G472">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="473" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A473" t="s">
+        <v>808</v>
+      </c>
+      <c r="B473" t="s">
+        <v>187</v>
+      </c>
+      <c r="C473" t="s">
+        <v>809</v>
+      </c>
+      <c r="D473" s="6" t="s">
+        <v>812</v>
+      </c>
+      <c r="E473">
+        <v>0</v>
+      </c>
+      <c r="F473">
+        <v>0</v>
+      </c>
+      <c r="G473">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="474" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A474" t="s">
+        <v>120</v>
+      </c>
+      <c r="B474" t="s">
+        <v>577</v>
+      </c>
+      <c r="C474" t="s">
+        <v>577</v>
+      </c>
+      <c r="D474" s="6" t="s">
+        <v>813</v>
+      </c>
+      <c r="E474">
+        <v>0</v>
+      </c>
+      <c r="F474">
+        <v>1</v>
+      </c>
+      <c r="G474">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A475" t="s">
+        <v>808</v>
+      </c>
+      <c r="B475" t="s">
+        <v>187</v>
+      </c>
+      <c r="C475" t="s">
+        <v>809</v>
+      </c>
+      <c r="D475" s="6" t="s">
+        <v>814</v>
+      </c>
+      <c r="E475">
+        <v>0</v>
+      </c>
+      <c r="F475">
+        <v>1</v>
+      </c>
+      <c r="G475">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A476" t="s">
+        <v>120</v>
+      </c>
+      <c r="B476" t="s">
+        <v>577</v>
+      </c>
+      <c r="C476" t="s">
+        <v>577</v>
+      </c>
+      <c r="D476" s="6" t="s">
+        <v>815</v>
+      </c>
+      <c r="E476">
+        <v>0</v>
+      </c>
+      <c r="F476">
+        <v>1</v>
+      </c>
+      <c r="G476">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="477" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A477" t="s">
+        <v>808</v>
+      </c>
+      <c r="B477" t="s">
+        <v>187</v>
+      </c>
+      <c r="C477" t="s">
+        <v>809</v>
+      </c>
+      <c r="D477" s="6" t="s">
+        <v>816</v>
+      </c>
+      <c r="E477">
+        <v>0</v>
+      </c>
+      <c r="F477">
+        <v>1</v>
+      </c>
+      <c r="G477">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="478" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A478" t="s">
         <v>121</v>
       </c>
-      <c r="B454" t="s">
+      <c r="B478" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="455" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A455" t="s">
+      <c r="C478" t="s">
+        <v>578</v>
+      </c>
+      <c r="D478" s="6" t="s">
+        <v>817</v>
+      </c>
+      <c r="E478">
+        <v>0</v>
+      </c>
+      <c r="F478">
+        <v>0</v>
+      </c>
+      <c r="G478">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="479" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A479" t="s">
+        <v>121</v>
+      </c>
+      <c r="B479" t="s">
+        <v>578</v>
+      </c>
+      <c r="C479" t="s">
+        <v>578</v>
+      </c>
+      <c r="D479" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="E479">
+        <v>0</v>
+      </c>
+      <c r="F479">
+        <v>0</v>
+      </c>
+      <c r="G479">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="480" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A480" t="s">
+        <v>121</v>
+      </c>
+      <c r="B480" t="s">
+        <v>578</v>
+      </c>
+      <c r="C480" t="s">
+        <v>578</v>
+      </c>
+      <c r="D480" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="E480">
+        <v>0</v>
+      </c>
+      <c r="F480">
+        <v>1</v>
+      </c>
+      <c r="G480">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A481" t="s">
+        <v>121</v>
+      </c>
+      <c r="B481" t="s">
+        <v>578</v>
+      </c>
+      <c r="C481" t="s">
+        <v>578</v>
+      </c>
+      <c r="D481" s="6" t="s">
+        <v>820</v>
+      </c>
+      <c r="E481">
+        <v>0</v>
+      </c>
+      <c r="F481">
+        <v>1</v>
+      </c>
+      <c r="G481">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A482" t="s">
+        <v>121</v>
+      </c>
+      <c r="B482" t="s">
+        <v>578</v>
+      </c>
+      <c r="C482" t="s">
+        <v>578</v>
+      </c>
+      <c r="D482" s="6" t="s">
+        <v>821</v>
+      </c>
+      <c r="E482">
+        <v>0</v>
+      </c>
+      <c r="F482">
+        <v>1</v>
+      </c>
+      <c r="G482">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="483" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A483" t="s">
         <v>579</v>
       </c>
-      <c r="B455" t="s">
+      <c r="B483" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="456" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A456" t="s">
+      <c r="C483" t="s">
+        <v>580</v>
+      </c>
+      <c r="D483" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="E483">
+        <v>1</v>
+      </c>
+      <c r="F483">
+        <v>0</v>
+      </c>
+      <c r="G483">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="484" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A484" t="s">
+        <v>579</v>
+      </c>
+      <c r="B484" t="s">
+        <v>580</v>
+      </c>
+      <c r="C484" t="s">
+        <v>580</v>
+      </c>
+      <c r="D484" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="E484">
+        <v>1</v>
+      </c>
+      <c r="F484">
+        <v>0</v>
+      </c>
+      <c r="G484">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="485" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A485" t="s">
+        <v>579</v>
+      </c>
+      <c r="B485" t="s">
+        <v>580</v>
+      </c>
+      <c r="C485" t="s">
+        <v>580</v>
+      </c>
+      <c r="D485" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="E485">
+        <v>1</v>
+      </c>
+      <c r="F485">
+        <v>1</v>
+      </c>
+      <c r="G485">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A486" t="s">
+        <v>579</v>
+      </c>
+      <c r="B486" t="s">
+        <v>580</v>
+      </c>
+      <c r="C486" t="s">
+        <v>580</v>
+      </c>
+      <c r="D486" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="E486">
+        <v>1</v>
+      </c>
+      <c r="F486">
+        <v>1</v>
+      </c>
+      <c r="G486">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="487" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A487" t="s">
+        <v>579</v>
+      </c>
+      <c r="B487" t="s">
+        <v>580</v>
+      </c>
+      <c r="C487" t="s">
+        <v>580</v>
+      </c>
+      <c r="D487" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="E487">
+        <v>1</v>
+      </c>
+      <c r="F487">
+        <v>1</v>
+      </c>
+      <c r="G487">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="488" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A488" t="s">
         <v>122</v>
       </c>
-      <c r="B456" t="s">
+      <c r="B488" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="457" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A457" t="s">
+      <c r="C488" t="s">
+        <v>581</v>
+      </c>
+      <c r="D488" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="E488">
+        <v>1</v>
+      </c>
+      <c r="F488">
+        <v>0</v>
+      </c>
+      <c r="G488">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="489" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A489" t="s">
+        <v>122</v>
+      </c>
+      <c r="B489" t="s">
+        <v>581</v>
+      </c>
+      <c r="C489" t="s">
+        <v>581</v>
+      </c>
+      <c r="D489" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="E489">
+        <v>1</v>
+      </c>
+      <c r="F489">
+        <v>0</v>
+      </c>
+      <c r="G489">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="490" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A490" t="s">
+        <v>122</v>
+      </c>
+      <c r="B490" t="s">
+        <v>581</v>
+      </c>
+      <c r="C490" t="s">
+        <v>581</v>
+      </c>
+      <c r="D490" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="E490">
+        <v>1</v>
+      </c>
+      <c r="F490">
+        <v>1</v>
+      </c>
+      <c r="G490">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="491" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A491" t="s">
+        <v>122</v>
+      </c>
+      <c r="B491" t="s">
+        <v>581</v>
+      </c>
+      <c r="C491" t="s">
+        <v>581</v>
+      </c>
+      <c r="D491" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="E491">
+        <v>1</v>
+      </c>
+      <c r="F491">
+        <v>1</v>
+      </c>
+      <c r="G491">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="492" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A492" t="s">
+        <v>122</v>
+      </c>
+      <c r="B492" t="s">
+        <v>581</v>
+      </c>
+      <c r="C492" t="s">
+        <v>581</v>
+      </c>
+      <c r="D492" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="E492">
+        <v>1</v>
+      </c>
+      <c r="F492">
+        <v>1</v>
+      </c>
+      <c r="G492">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="493" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A493" t="s">
         <v>123</v>
       </c>
-      <c r="B457" t="s">
+      <c r="B493" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="458" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A458" t="s">
-        <v>124</v>
-      </c>
-      <c r="B458" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="459" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A459" t="s">
-        <v>125</v>
-      </c>
-      <c r="B459" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="460" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A460" t="s">
-        <v>126</v>
-      </c>
-      <c r="B460" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="461" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A461" t="s">
-        <v>127</v>
-      </c>
-      <c r="B461" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="462" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A462" t="s">
-        <v>128</v>
-      </c>
-      <c r="B462" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="463" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A463" t="s">
-        <v>129</v>
-      </c>
-      <c r="B463" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="464" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A464" t="s">
-        <v>130</v>
-      </c>
-      <c r="B464" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="465" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A465" t="s">
-        <v>131</v>
-      </c>
-      <c r="B465" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="466" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A466" t="s">
-        <v>592</v>
-      </c>
-      <c r="B466" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="467" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A467" t="s">
-        <v>132</v>
-      </c>
-      <c r="B467" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="468" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A468" t="s">
-        <v>133</v>
-      </c>
-      <c r="B468" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="469" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A469" t="s">
-        <v>134</v>
-      </c>
-      <c r="B469" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="470" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A470" t="s">
-        <v>135</v>
-      </c>
-      <c r="B470" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="471" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A471" t="s">
-        <v>136</v>
-      </c>
-      <c r="B471" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="472" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A472" t="s">
-        <v>137</v>
-      </c>
-      <c r="B472" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="473" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A473" t="s">
-        <v>138</v>
-      </c>
-      <c r="B473" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="474" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A474" t="s">
-        <v>139</v>
-      </c>
-      <c r="B474" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="475" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A475" t="s">
-        <v>140</v>
-      </c>
-      <c r="B475" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="476" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A476" t="s">
-        <v>141</v>
-      </c>
-      <c r="B476" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="477" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A477" t="s">
-        <v>142</v>
-      </c>
-      <c r="B477" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="478" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A478" t="s">
-        <v>143</v>
-      </c>
-      <c r="B478" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="479" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A479" t="s">
-        <v>144</v>
-      </c>
-      <c r="B479" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A480" t="s">
-        <v>145</v>
-      </c>
-      <c r="B480" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A481" t="s">
-        <v>146</v>
-      </c>
-      <c r="B481" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="482" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A482" t="s">
-        <v>147</v>
-      </c>
-      <c r="B482" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="483" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A483" t="s">
-        <v>148</v>
-      </c>
-      <c r="B483" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="484" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A484" t="s">
-        <v>149</v>
-      </c>
-      <c r="B484" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="485" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A485" t="s">
-        <v>150</v>
-      </c>
-      <c r="B485" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="486" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A486" t="s">
-        <v>151</v>
-      </c>
-      <c r="B486" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="487" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A487" t="s">
-        <v>152</v>
-      </c>
-      <c r="B487" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="488" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A488" t="s">
-        <v>153</v>
-      </c>
-      <c r="B488" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="489" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A489" t="s">
-        <v>154</v>
-      </c>
-      <c r="B489" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="490" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A490" t="s">
-        <v>155</v>
-      </c>
-      <c r="B490" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="491" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A491" t="s">
-        <v>156</v>
-      </c>
-      <c r="B491" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="492" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A492" t="s">
-        <v>157</v>
-      </c>
-      <c r="B492" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="493" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A493" t="s">
-        <v>158</v>
-      </c>
-      <c r="B493" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="494" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C493" t="s">
+        <v>582</v>
+      </c>
+      <c r="D493" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="E493">
+        <v>1</v>
+      </c>
+      <c r="F493">
+        <v>0</v>
+      </c>
+      <c r="G493">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="494" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="B494" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="495" spans="1:2" x14ac:dyDescent="0.2">
+        <v>582</v>
+      </c>
+      <c r="C494" t="s">
+        <v>582</v>
+      </c>
+      <c r="D494" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="E494">
+        <v>1</v>
+      </c>
+      <c r="F494">
+        <v>0</v>
+      </c>
+      <c r="G494">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="495" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
       <c r="B495" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="496" spans="1:2" x14ac:dyDescent="0.2">
+        <v>582</v>
+      </c>
+      <c r="C495" t="s">
+        <v>582</v>
+      </c>
+      <c r="D495" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="E495">
+        <v>1</v>
+      </c>
+      <c r="F495">
+        <v>1</v>
+      </c>
+      <c r="G495">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="496" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="B496" t="s">
-        <v>619</v>
+        <v>582</v>
+      </c>
+      <c r="C496" t="s">
+        <v>582</v>
+      </c>
+      <c r="D496" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="E496">
+        <v>1</v>
+      </c>
+      <c r="F496">
+        <v>1</v>
+      </c>
+      <c r="G496">
+        <v>0</v>
       </c>
     </row>
     <row r="497" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
-        <v>162</v>
+        <v>123</v>
       </c>
       <c r="B497" t="s">
-        <v>569</v>
+        <v>582</v>
+      </c>
+      <c r="C497" t="s">
+        <v>582</v>
+      </c>
+      <c r="D497" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="E497">
+        <v>1</v>
+      </c>
+      <c r="F497">
+        <v>1</v>
+      </c>
+      <c r="G497">
+        <v>0</v>
       </c>
     </row>
     <row r="498" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A498" t="s">
-        <v>163</v>
+        <v>124</v>
+      </c>
+      <c r="B498" t="s">
+        <v>583</v>
+      </c>
+      <c r="C498" t="s">
+        <v>583</v>
+      </c>
+      <c r="D498" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="E498">
+        <v>1</v>
+      </c>
+      <c r="F498">
+        <v>0</v>
+      </c>
+      <c r="G498">
+        <v>0</v>
       </c>
     </row>
     <row r="499" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A499" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="B499" t="s">
-        <v>620</v>
+        <v>583</v>
+      </c>
+      <c r="C499" t="s">
+        <v>583</v>
+      </c>
+      <c r="D499" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="E499">
+        <v>1</v>
+      </c>
+      <c r="F499">
+        <v>0</v>
+      </c>
+      <c r="G499">
+        <v>1</v>
       </c>
     </row>
     <row r="500" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="B500" t="s">
-        <v>621</v>
+        <v>583</v>
       </c>
       <c r="C500" t="s">
-        <v>498</v>
+        <v>583</v>
       </c>
       <c r="D500" s="6" t="s">
-        <v>499</v>
+        <v>824</v>
       </c>
       <c r="E500">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F500">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G500">
         <v>0</v>
@@ -13662,22 +14757,22 @@
     </row>
     <row r="501" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="B501" t="s">
-        <v>621</v>
+        <v>583</v>
       </c>
       <c r="C501" t="s">
-        <v>498</v>
+        <v>583</v>
       </c>
       <c r="D501" s="6" t="s">
-        <v>190</v>
+        <v>825</v>
       </c>
       <c r="E501">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F501">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G501">
         <v>0</v>
@@ -13685,158 +14780,1969 @@
     </row>
     <row r="502" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
-        <v>166</v>
+        <v>124</v>
       </c>
       <c r="B502" t="s">
-        <v>622</v>
+        <v>583</v>
+      </c>
+      <c r="C502" t="s">
+        <v>583</v>
+      </c>
+      <c r="D502" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="E502">
+        <v>1</v>
+      </c>
+      <c r="F502">
+        <v>1</v>
+      </c>
+      <c r="G502">
+        <v>0</v>
       </c>
     </row>
     <row r="503" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
-        <v>167</v>
+        <v>125</v>
       </c>
       <c r="B503" t="s">
-        <v>623</v>
+        <v>584</v>
+      </c>
+      <c r="C503" t="s">
+        <v>187</v>
+      </c>
+      <c r="D503" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E503" t="s">
+        <v>187</v>
+      </c>
+      <c r="F503" t="s">
+        <v>187</v>
+      </c>
+      <c r="G503" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="504" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
-        <v>168</v>
+        <v>126</v>
       </c>
       <c r="B504" t="s">
-        <v>624</v>
+        <v>588</v>
+      </c>
+      <c r="C504" t="s">
+        <v>588</v>
+      </c>
+      <c r="D504" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="E504">
+        <v>1</v>
+      </c>
+      <c r="F504">
+        <v>0</v>
+      </c>
+      <c r="G504">
+        <v>0</v>
       </c>
     </row>
     <row r="505" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
-        <v>169</v>
+        <v>126</v>
       </c>
       <c r="B505" t="s">
-        <v>187</v>
+        <v>588</v>
+      </c>
+      <c r="C505" t="s">
+        <v>588</v>
+      </c>
+      <c r="D505" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="E505">
+        <v>1</v>
+      </c>
+      <c r="F505">
+        <v>0</v>
+      </c>
+      <c r="G505">
+        <v>1</v>
       </c>
     </row>
     <row r="506" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A506" s="12" t="s">
-        <v>170</v>
+      <c r="A506" t="s">
+        <v>126</v>
       </c>
       <c r="B506" t="s">
-        <v>625</v>
+        <v>588</v>
+      </c>
+      <c r="C506" t="s">
+        <v>588</v>
+      </c>
+      <c r="D506" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="E506">
+        <v>1</v>
+      </c>
+      <c r="F506">
+        <v>1</v>
+      </c>
+      <c r="G506">
+        <v>0</v>
       </c>
     </row>
     <row r="507" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="B507" t="s">
-        <v>626</v>
+        <v>588</v>
+      </c>
+      <c r="C507" t="s">
+        <v>588</v>
+      </c>
+      <c r="D507" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="E507">
+        <v>1</v>
+      </c>
+      <c r="F507">
+        <v>1</v>
+      </c>
+      <c r="G507">
+        <v>0</v>
       </c>
     </row>
     <row r="508" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A508" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
       <c r="B508" t="s">
-        <v>576</v>
+        <v>588</v>
+      </c>
+      <c r="C508" t="s">
+        <v>588</v>
+      </c>
+      <c r="D508" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="E508">
+        <v>1</v>
+      </c>
+      <c r="F508">
+        <v>1</v>
+      </c>
+      <c r="G508">
+        <v>0</v>
       </c>
     </row>
     <row r="509" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A509" t="s">
-        <v>173</v>
+        <v>127</v>
       </c>
       <c r="B509" t="s">
-        <v>627</v>
+        <v>589</v>
+      </c>
+      <c r="C509" t="s">
+        <v>187</v>
+      </c>
+      <c r="D509" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E509" t="s">
+        <v>187</v>
+      </c>
+      <c r="F509" t="s">
+        <v>187</v>
+      </c>
+      <c r="G509" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="510" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A510" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="B510" t="s">
-        <v>628</v>
+        <v>590</v>
+      </c>
+      <c r="C510" t="s">
+        <v>187</v>
+      </c>
+      <c r="D510" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E510" t="s">
+        <v>187</v>
+      </c>
+      <c r="F510" t="s">
+        <v>187</v>
+      </c>
+      <c r="G510" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="511" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A511" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="B511" t="s">
-        <v>629</v>
+        <v>585</v>
+      </c>
+      <c r="C511" t="s">
+        <v>585</v>
+      </c>
+      <c r="D511" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="E511">
+        <v>1</v>
+      </c>
+      <c r="F511">
+        <v>0</v>
+      </c>
+      <c r="G511">
+        <v>0</v>
       </c>
     </row>
     <row r="512" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A512" t="s">
+        <v>129</v>
+      </c>
+      <c r="B512" t="s">
+        <v>585</v>
+      </c>
+      <c r="C512" t="s">
+        <v>585</v>
+      </c>
+      <c r="D512" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="E512">
+        <v>1</v>
+      </c>
+      <c r="F512">
+        <v>0</v>
+      </c>
+      <c r="G512">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A513" t="s">
+        <v>129</v>
+      </c>
+      <c r="B513" t="s">
+        <v>585</v>
+      </c>
+      <c r="C513" t="s">
+        <v>585</v>
+      </c>
+      <c r="D513" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="E513">
+        <v>1</v>
+      </c>
+      <c r="F513">
+        <v>1</v>
+      </c>
+      <c r="G513">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="514" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A514" t="s">
+        <v>129</v>
+      </c>
+      <c r="B514" t="s">
+        <v>585</v>
+      </c>
+      <c r="C514" t="s">
+        <v>585</v>
+      </c>
+      <c r="D514" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="E514">
+        <v>1</v>
+      </c>
+      <c r="F514">
+        <v>1</v>
+      </c>
+      <c r="G514">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="515" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A515" t="s">
+        <v>129</v>
+      </c>
+      <c r="B515" t="s">
+        <v>585</v>
+      </c>
+      <c r="C515" t="s">
+        <v>585</v>
+      </c>
+      <c r="D515" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="E515">
+        <v>1</v>
+      </c>
+      <c r="F515">
+        <v>1</v>
+      </c>
+      <c r="G515">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="516" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A516" t="s">
+        <v>130</v>
+      </c>
+      <c r="B516" t="s">
+        <v>586</v>
+      </c>
+      <c r="C516" t="s">
+        <v>586</v>
+      </c>
+      <c r="D516" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="E516">
+        <v>1</v>
+      </c>
+      <c r="F516">
+        <v>0</v>
+      </c>
+      <c r="G516">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="517" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A517" t="s">
+        <v>130</v>
+      </c>
+      <c r="B517" t="s">
+        <v>586</v>
+      </c>
+      <c r="C517" t="s">
+        <v>586</v>
+      </c>
+      <c r="D517" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="E517">
+        <v>1</v>
+      </c>
+      <c r="F517">
+        <v>0</v>
+      </c>
+      <c r="G517">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="518" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A518" t="s">
+        <v>130</v>
+      </c>
+      <c r="B518" t="s">
+        <v>586</v>
+      </c>
+      <c r="C518" t="s">
+        <v>586</v>
+      </c>
+      <c r="D518" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="E518">
+        <v>1</v>
+      </c>
+      <c r="F518">
+        <v>1</v>
+      </c>
+      <c r="G518">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="519" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A519" t="s">
+        <v>130</v>
+      </c>
+      <c r="B519" t="s">
+        <v>586</v>
+      </c>
+      <c r="C519" t="s">
+        <v>586</v>
+      </c>
+      <c r="D519" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="E519">
+        <v>1</v>
+      </c>
+      <c r="F519">
+        <v>1</v>
+      </c>
+      <c r="G519">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="520" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A520" t="s">
+        <v>130</v>
+      </c>
+      <c r="B520" t="s">
+        <v>586</v>
+      </c>
+      <c r="C520" t="s">
+        <v>586</v>
+      </c>
+      <c r="D520" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="E520">
+        <v>1</v>
+      </c>
+      <c r="F520">
+        <v>1</v>
+      </c>
+      <c r="G520">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="521" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A521" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B521" t="s">
+        <v>587</v>
+      </c>
+      <c r="C521" t="s">
+        <v>587</v>
+      </c>
+      <c r="D521" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="E521">
+        <v>1</v>
+      </c>
+      <c r="F521">
+        <v>0</v>
+      </c>
+      <c r="G521">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="522" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A522" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B522" t="s">
+        <v>587</v>
+      </c>
+      <c r="C522" t="s">
+        <v>587</v>
+      </c>
+      <c r="D522" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="E522">
+        <v>1</v>
+      </c>
+      <c r="F522">
+        <v>0</v>
+      </c>
+      <c r="G522">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="523" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A523" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B523" t="s">
+        <v>587</v>
+      </c>
+      <c r="C523" t="s">
+        <v>587</v>
+      </c>
+      <c r="D523" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="E523">
+        <v>1</v>
+      </c>
+      <c r="F523">
+        <v>1</v>
+      </c>
+      <c r="G523">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="524" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A524" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B524" t="s">
+        <v>587</v>
+      </c>
+      <c r="C524" t="s">
+        <v>587</v>
+      </c>
+      <c r="D524" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="E524">
+        <v>1</v>
+      </c>
+      <c r="F524">
+        <v>1</v>
+      </c>
+      <c r="G524">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="525" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A525" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B525" t="s">
+        <v>587</v>
+      </c>
+      <c r="C525" t="s">
+        <v>587</v>
+      </c>
+      <c r="D525" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="E525">
+        <v>1</v>
+      </c>
+      <c r="F525">
+        <v>1</v>
+      </c>
+      <c r="G525">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="526" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A526" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="B526" t="s">
+        <v>593</v>
+      </c>
+      <c r="C526" t="s">
+        <v>593</v>
+      </c>
+      <c r="D526" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="E526">
+        <v>0</v>
+      </c>
+      <c r="F526">
+        <v>0</v>
+      </c>
+      <c r="G526">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="527" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A527" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="B527" t="s">
+        <v>593</v>
+      </c>
+      <c r="C527" t="s">
+        <v>593</v>
+      </c>
+      <c r="D527" s="6" t="s">
+        <v>828</v>
+      </c>
+      <c r="E527">
+        <v>0</v>
+      </c>
+      <c r="F527">
+        <v>0</v>
+      </c>
+      <c r="G527">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="528" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A528" t="s">
+        <v>132</v>
+      </c>
+      <c r="B528" t="s">
+        <v>594</v>
+      </c>
+      <c r="C528" t="s">
+        <v>594</v>
+      </c>
+      <c r="D528" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="E528">
+        <v>0</v>
+      </c>
+      <c r="F528">
+        <v>0</v>
+      </c>
+      <c r="G528">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="529" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A529" t="s">
+        <v>132</v>
+      </c>
+      <c r="B529" t="s">
+        <v>594</v>
+      </c>
+      <c r="C529" t="s">
+        <v>594</v>
+      </c>
+      <c r="D529" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="E529">
+        <v>0</v>
+      </c>
+      <c r="F529">
+        <v>0</v>
+      </c>
+      <c r="G529">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="530" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A530" t="s">
+        <v>133</v>
+      </c>
+      <c r="B530" t="s">
+        <v>596</v>
+      </c>
+      <c r="C530" t="s">
+        <v>596</v>
+      </c>
+      <c r="D530" s="6" t="s">
+        <v>831</v>
+      </c>
+      <c r="E530">
+        <v>0</v>
+      </c>
+      <c r="F530">
+        <v>0</v>
+      </c>
+      <c r="G530">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="531" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A531" t="s">
+        <v>133</v>
+      </c>
+      <c r="B531" t="s">
+        <v>596</v>
+      </c>
+      <c r="C531" t="s">
+        <v>596</v>
+      </c>
+      <c r="D531" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="E531">
+        <v>0</v>
+      </c>
+      <c r="F531">
+        <v>0</v>
+      </c>
+      <c r="G531">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="532" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A532" t="s">
+        <v>133</v>
+      </c>
+      <c r="B532" t="s">
+        <v>596</v>
+      </c>
+      <c r="C532" t="s">
+        <v>596</v>
+      </c>
+      <c r="D532" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="E532">
+        <v>0</v>
+      </c>
+      <c r="F532">
+        <v>1</v>
+      </c>
+      <c r="G532">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="533" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A533" t="s">
+        <v>133</v>
+      </c>
+      <c r="B533" t="s">
+        <v>596</v>
+      </c>
+      <c r="C533" t="s">
+        <v>596</v>
+      </c>
+      <c r="D533" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="E533">
+        <v>0</v>
+      </c>
+      <c r="F533">
+        <v>1</v>
+      </c>
+      <c r="G533">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="534" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A534" t="s">
+        <v>134</v>
+      </c>
+      <c r="B534" t="s">
+        <v>597</v>
+      </c>
+      <c r="C534" t="s">
+        <v>597</v>
+      </c>
+      <c r="D534" s="6" t="s">
+        <v>835</v>
+      </c>
+      <c r="E534">
+        <v>0</v>
+      </c>
+      <c r="F534">
+        <v>0</v>
+      </c>
+      <c r="G534">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="535" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A535" t="s">
+        <v>134</v>
+      </c>
+      <c r="B535" t="s">
+        <v>597</v>
+      </c>
+      <c r="C535" t="s">
+        <v>597</v>
+      </c>
+      <c r="D535" s="6" t="s">
+        <v>836</v>
+      </c>
+      <c r="E535">
+        <v>0</v>
+      </c>
+      <c r="F535">
+        <v>0</v>
+      </c>
+      <c r="G535">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="536" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A536" t="s">
+        <v>134</v>
+      </c>
+      <c r="B536" t="s">
+        <v>597</v>
+      </c>
+      <c r="C536" t="s">
+        <v>597</v>
+      </c>
+      <c r="D536" s="6" t="s">
+        <v>837</v>
+      </c>
+      <c r="E536">
+        <v>0</v>
+      </c>
+      <c r="F536">
+        <v>1</v>
+      </c>
+      <c r="G536">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="537" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A537" t="s">
+        <v>134</v>
+      </c>
+      <c r="B537" t="s">
+        <v>597</v>
+      </c>
+      <c r="C537" t="s">
+        <v>597</v>
+      </c>
+      <c r="D537" s="6" t="s">
+        <v>838</v>
+      </c>
+      <c r="E537">
+        <v>0</v>
+      </c>
+      <c r="F537">
+        <v>1</v>
+      </c>
+      <c r="G537">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="538" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A538" t="s">
+        <v>135</v>
+      </c>
+      <c r="B538" t="s">
+        <v>598</v>
+      </c>
+      <c r="C538" t="s">
+        <v>187</v>
+      </c>
+      <c r="D538" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E538" t="s">
+        <v>187</v>
+      </c>
+      <c r="F538" t="s">
+        <v>187</v>
+      </c>
+      <c r="G538" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="539" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A539" t="s">
+        <v>136</v>
+      </c>
+      <c r="B539" t="s">
+        <v>599</v>
+      </c>
+      <c r="C539" t="s">
+        <v>187</v>
+      </c>
+      <c r="D539" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E539" t="s">
+        <v>187</v>
+      </c>
+      <c r="F539" t="s">
+        <v>187</v>
+      </c>
+      <c r="G539" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="540" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A540" t="s">
+        <v>137</v>
+      </c>
+      <c r="B540" t="s">
+        <v>600</v>
+      </c>
+      <c r="C540" t="s">
+        <v>187</v>
+      </c>
+      <c r="D540" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E540" t="s">
+        <v>187</v>
+      </c>
+      <c r="F540" t="s">
+        <v>187</v>
+      </c>
+      <c r="G540" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="541" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A541" t="s">
+        <v>138</v>
+      </c>
+      <c r="B541" t="s">
+        <v>601</v>
+      </c>
+      <c r="C541" t="s">
+        <v>601</v>
+      </c>
+      <c r="D541" s="6" t="s">
+        <v>839</v>
+      </c>
+      <c r="E541">
+        <v>0</v>
+      </c>
+      <c r="F541">
+        <v>0</v>
+      </c>
+      <c r="G541">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="542" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A542" t="s">
+        <v>138</v>
+      </c>
+      <c r="B542" t="s">
+        <v>601</v>
+      </c>
+      <c r="C542" t="s">
+        <v>601</v>
+      </c>
+      <c r="D542" s="6" t="s">
+        <v>840</v>
+      </c>
+      <c r="E542">
+        <v>0</v>
+      </c>
+      <c r="F542">
+        <v>0</v>
+      </c>
+      <c r="G542">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="543" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A543" t="s">
+        <v>139</v>
+      </c>
+      <c r="B543" t="s">
+        <v>602</v>
+      </c>
+      <c r="C543" t="s">
+        <v>602</v>
+      </c>
+      <c r="D543" s="6" t="s">
+        <v>841</v>
+      </c>
+      <c r="E543">
+        <v>0</v>
+      </c>
+      <c r="F543">
+        <v>0</v>
+      </c>
+      <c r="G543">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="544" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A544" t="s">
+        <v>139</v>
+      </c>
+      <c r="B544" t="s">
+        <v>602</v>
+      </c>
+      <c r="C544" t="s">
+        <v>602</v>
+      </c>
+      <c r="D544" s="6" t="s">
+        <v>842</v>
+      </c>
+      <c r="E544">
+        <v>0</v>
+      </c>
+      <c r="F544">
+        <v>0</v>
+      </c>
+      <c r="G544">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="545" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A545" t="s">
+        <v>139</v>
+      </c>
+      <c r="B545" t="s">
+        <v>602</v>
+      </c>
+      <c r="C545" t="s">
+        <v>602</v>
+      </c>
+      <c r="D545" s="6" t="s">
+        <v>843</v>
+      </c>
+      <c r="E545">
+        <v>0</v>
+      </c>
+      <c r="F545">
+        <v>0</v>
+      </c>
+      <c r="G545">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="546" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A546" t="s">
+        <v>140</v>
+      </c>
+      <c r="B546" t="s">
+        <v>187</v>
+      </c>
+      <c r="C546" t="s">
+        <v>187</v>
+      </c>
+      <c r="D546" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E546" t="s">
+        <v>187</v>
+      </c>
+      <c r="F546" t="s">
+        <v>187</v>
+      </c>
+      <c r="G546" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="547" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A547" t="s">
+        <v>141</v>
+      </c>
+      <c r="B547" t="s">
+        <v>603</v>
+      </c>
+      <c r="C547" t="s">
+        <v>603</v>
+      </c>
+      <c r="D547" s="6" t="s">
+        <v>844</v>
+      </c>
+      <c r="E547">
+        <v>0</v>
+      </c>
+      <c r="F547">
+        <v>0</v>
+      </c>
+      <c r="G547">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="548" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A548" t="s">
+        <v>141</v>
+      </c>
+      <c r="B548" t="s">
+        <v>603</v>
+      </c>
+      <c r="C548" t="s">
+        <v>603</v>
+      </c>
+      <c r="D548" s="6" t="s">
+        <v>845</v>
+      </c>
+      <c r="E548">
+        <v>0</v>
+      </c>
+      <c r="F548">
+        <v>0</v>
+      </c>
+      <c r="G548">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="549" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A549" t="s">
+        <v>141</v>
+      </c>
+      <c r="B549" t="s">
+        <v>603</v>
+      </c>
+      <c r="C549" t="s">
+        <v>603</v>
+      </c>
+      <c r="D549" s="6" t="s">
+        <v>846</v>
+      </c>
+      <c r="E549">
+        <v>0</v>
+      </c>
+      <c r="F549">
+        <v>0</v>
+      </c>
+      <c r="G549">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="550" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A550" t="s">
+        <v>142</v>
+      </c>
+      <c r="B550" t="s">
+        <v>604</v>
+      </c>
+      <c r="C550" t="s">
+        <v>604</v>
+      </c>
+      <c r="D550" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="E550">
+        <v>1</v>
+      </c>
+      <c r="F550">
+        <v>0</v>
+      </c>
+      <c r="G550">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="551" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A551" t="s">
+        <v>142</v>
+      </c>
+      <c r="B551" t="s">
+        <v>604</v>
+      </c>
+      <c r="C551" t="s">
+        <v>604</v>
+      </c>
+      <c r="D551" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="E551">
+        <v>1</v>
+      </c>
+      <c r="F551">
+        <v>0</v>
+      </c>
+      <c r="G551">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="552" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A552" t="s">
+        <v>142</v>
+      </c>
+      <c r="B552" t="s">
+        <v>604</v>
+      </c>
+      <c r="C552" t="s">
+        <v>604</v>
+      </c>
+      <c r="D552" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="E552">
+        <v>1</v>
+      </c>
+      <c r="F552">
+        <v>0</v>
+      </c>
+      <c r="G552">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="553" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A553" t="s">
+        <v>142</v>
+      </c>
+      <c r="B553" t="s">
+        <v>604</v>
+      </c>
+      <c r="C553" t="s">
+        <v>604</v>
+      </c>
+      <c r="D553" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="E553">
+        <v>1</v>
+      </c>
+      <c r="F553">
+        <v>0</v>
+      </c>
+      <c r="G553">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="554" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A554" t="s">
+        <v>142</v>
+      </c>
+      <c r="B554" t="s">
+        <v>604</v>
+      </c>
+      <c r="C554" t="s">
+        <v>604</v>
+      </c>
+      <c r="D554" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="E554">
+        <v>1</v>
+      </c>
+      <c r="F554">
+        <v>0</v>
+      </c>
+      <c r="G554">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="555" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A555" t="s">
+        <v>142</v>
+      </c>
+      <c r="B555" t="s">
+        <v>604</v>
+      </c>
+      <c r="C555" t="s">
+        <v>604</v>
+      </c>
+      <c r="D555" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="E555">
+        <v>1</v>
+      </c>
+      <c r="F555">
+        <v>0</v>
+      </c>
+      <c r="G555">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="556" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A556" t="s">
+        <v>143</v>
+      </c>
+      <c r="B556" t="s">
+        <v>605</v>
+      </c>
+      <c r="C556" t="s">
+        <v>187</v>
+      </c>
+      <c r="D556" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E556" t="s">
+        <v>187</v>
+      </c>
+      <c r="F556" t="s">
+        <v>187</v>
+      </c>
+      <c r="G556" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="557" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A557" t="s">
+        <v>144</v>
+      </c>
+      <c r="B557" t="s">
+        <v>606</v>
+      </c>
+      <c r="C557" t="s">
+        <v>606</v>
+      </c>
+      <c r="D557" s="6" t="s">
+        <v>847</v>
+      </c>
+      <c r="E557">
+        <v>0</v>
+      </c>
+      <c r="F557">
+        <v>0</v>
+      </c>
+      <c r="G557">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="558" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A558" t="s">
+        <v>144</v>
+      </c>
+      <c r="B558" t="s">
+        <v>606</v>
+      </c>
+      <c r="C558" t="s">
+        <v>606</v>
+      </c>
+      <c r="D558" s="6" t="s">
+        <v>848</v>
+      </c>
+      <c r="E558">
+        <v>0</v>
+      </c>
+      <c r="F558">
+        <v>0</v>
+      </c>
+      <c r="G558">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="559" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A559" t="s">
+        <v>144</v>
+      </c>
+      <c r="B559" t="s">
+        <v>606</v>
+      </c>
+      <c r="C559" t="s">
+        <v>606</v>
+      </c>
+      <c r="D559" s="6" t="s">
+        <v>849</v>
+      </c>
+      <c r="E559">
+        <v>0</v>
+      </c>
+      <c r="F559">
+        <v>0</v>
+      </c>
+      <c r="G559">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="560" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A560" t="s">
+        <v>144</v>
+      </c>
+      <c r="B560" t="s">
+        <v>606</v>
+      </c>
+      <c r="C560" t="s">
+        <v>606</v>
+      </c>
+      <c r="D560" s="6" t="s">
+        <v>850</v>
+      </c>
+      <c r="E560">
+        <v>0</v>
+      </c>
+      <c r="F560">
+        <v>0</v>
+      </c>
+      <c r="G560">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="561" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A561" t="s">
+        <v>144</v>
+      </c>
+      <c r="B561" t="s">
+        <v>606</v>
+      </c>
+      <c r="C561" t="s">
+        <v>606</v>
+      </c>
+      <c r="D561" s="6" t="s">
+        <v>851</v>
+      </c>
+      <c r="E561">
+        <v>0</v>
+      </c>
+      <c r="F561">
+        <v>0</v>
+      </c>
+      <c r="G561">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="562" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A562" t="s">
+        <v>144</v>
+      </c>
+      <c r="B562" t="s">
+        <v>606</v>
+      </c>
+      <c r="C562" t="s">
+        <v>606</v>
+      </c>
+      <c r="D562" s="6" t="s">
+        <v>852</v>
+      </c>
+      <c r="E562">
+        <v>0</v>
+      </c>
+      <c r="F562">
+        <v>0</v>
+      </c>
+      <c r="G562">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="563" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A563" t="s">
+        <v>144</v>
+      </c>
+      <c r="B563" t="s">
+        <v>606</v>
+      </c>
+      <c r="C563" t="s">
+        <v>606</v>
+      </c>
+      <c r="D563" s="6" t="s">
+        <v>853</v>
+      </c>
+      <c r="E563">
+        <v>0</v>
+      </c>
+      <c r="F563">
+        <v>0</v>
+      </c>
+      <c r="G563">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="564" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A564" t="s">
+        <v>144</v>
+      </c>
+      <c r="B564" t="s">
+        <v>606</v>
+      </c>
+      <c r="C564" t="s">
+        <v>606</v>
+      </c>
+      <c r="D564" s="6" t="s">
+        <v>854</v>
+      </c>
+      <c r="E564">
+        <v>0</v>
+      </c>
+      <c r="F564">
+        <v>0</v>
+      </c>
+      <c r="G564">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="565" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A565" t="s">
+        <v>144</v>
+      </c>
+      <c r="B565" t="s">
+        <v>606</v>
+      </c>
+      <c r="C565" t="s">
+        <v>606</v>
+      </c>
+      <c r="D565" s="6" t="s">
+        <v>855</v>
+      </c>
+      <c r="E565">
+        <v>0</v>
+      </c>
+      <c r="F565">
+        <v>0</v>
+      </c>
+      <c r="G565">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="566" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A566" t="s">
+        <v>145</v>
+      </c>
+      <c r="B566" t="s">
+        <v>607</v>
+      </c>
+      <c r="C566" t="s">
+        <v>187</v>
+      </c>
+      <c r="D566" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E566" t="s">
+        <v>187</v>
+      </c>
+      <c r="F566" t="s">
+        <v>187</v>
+      </c>
+      <c r="G566" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="567" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A567" t="s">
+        <v>146</v>
+      </c>
+      <c r="B567" t="s">
+        <v>546</v>
+      </c>
+      <c r="C567" t="s">
+        <v>541</v>
+      </c>
+      <c r="D567" s="6" t="s">
+        <v>760</v>
+      </c>
+      <c r="E567">
+        <v>1</v>
+      </c>
+      <c r="F567">
+        <v>0</v>
+      </c>
+      <c r="G567">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="568" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A568" t="s">
+        <v>147</v>
+      </c>
+      <c r="B568" t="s">
+        <v>562</v>
+      </c>
+      <c r="C568" t="s">
+        <v>857</v>
+      </c>
+      <c r="D568" s="6" t="s">
+        <v>856</v>
+      </c>
+      <c r="E568">
+        <v>1</v>
+      </c>
+      <c r="F568">
+        <v>0</v>
+      </c>
+      <c r="G568">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="569" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A569" t="s">
+        <v>147</v>
+      </c>
+      <c r="B569" t="s">
+        <v>562</v>
+      </c>
+      <c r="C569" t="s">
+        <v>857</v>
+      </c>
+      <c r="D569" s="6" t="s">
+        <v>858</v>
+      </c>
+      <c r="E569">
+        <v>1</v>
+      </c>
+      <c r="F569">
+        <v>0</v>
+      </c>
+      <c r="G569">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="570" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A570" t="s">
+        <v>148</v>
+      </c>
+      <c r="B570" t="s">
+        <v>568</v>
+      </c>
+      <c r="C570" t="s">
+        <v>187</v>
+      </c>
+      <c r="D570" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E570" t="s">
+        <v>187</v>
+      </c>
+      <c r="F570" t="s">
+        <v>187</v>
+      </c>
+      <c r="G570" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="571" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A571" t="s">
+        <v>149</v>
+      </c>
+      <c r="B571" t="s">
+        <v>595</v>
+      </c>
+      <c r="C571" t="s">
+        <v>595</v>
+      </c>
+      <c r="D571" s="6" t="s">
+        <v>859</v>
+      </c>
+      <c r="E571">
+        <v>0</v>
+      </c>
+      <c r="F571">
+        <v>0</v>
+      </c>
+      <c r="G571">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="572" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A572" t="s">
+        <v>149</v>
+      </c>
+      <c r="B572" t="s">
+        <v>595</v>
+      </c>
+      <c r="C572" t="s">
+        <v>595</v>
+      </c>
+      <c r="D572" s="6" t="s">
+        <v>860</v>
+      </c>
+      <c r="E572">
+        <v>0</v>
+      </c>
+      <c r="F572">
+        <v>0</v>
+      </c>
+      <c r="G572">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="573" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A573" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B573" t="s">
+        <v>608</v>
+      </c>
+      <c r="C573" t="s">
+        <v>187</v>
+      </c>
+      <c r="D573" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E573" t="s">
+        <v>187</v>
+      </c>
+      <c r="F573" t="s">
+        <v>187</v>
+      </c>
+      <c r="G573" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="574" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A574" t="s">
+        <v>151</v>
+      </c>
+      <c r="B574" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="575" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A575" t="s">
+        <v>152</v>
+      </c>
+      <c r="B575" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="576" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A576" t="s">
+        <v>153</v>
+      </c>
+      <c r="B576" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="577" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A577" t="s">
+        <v>154</v>
+      </c>
+      <c r="B577" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="578" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A578" t="s">
+        <v>155</v>
+      </c>
+      <c r="B578" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="579" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A579" t="s">
+        <v>156</v>
+      </c>
+      <c r="B579" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="580" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A580" t="s">
+        <v>157</v>
+      </c>
+      <c r="B580" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="581" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A581" t="s">
+        <v>158</v>
+      </c>
+      <c r="B581" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="582" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A582" t="s">
+        <v>159</v>
+      </c>
+      <c r="B582" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="583" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A583" t="s">
+        <v>160</v>
+      </c>
+      <c r="B583" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="584" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A584" t="s">
+        <v>161</v>
+      </c>
+      <c r="B584" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="585" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A585" t="s">
+        <v>162</v>
+      </c>
+      <c r="B585" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="586" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A586" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="587" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A587" t="s">
+        <v>164</v>
+      </c>
+      <c r="B587" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="588" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A588" t="s">
+        <v>165</v>
+      </c>
+      <c r="B588" t="s">
+        <v>621</v>
+      </c>
+      <c r="C588" t="s">
+        <v>498</v>
+      </c>
+      <c r="D588" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="E588">
+        <v>0</v>
+      </c>
+      <c r="F588">
+        <v>0</v>
+      </c>
+      <c r="G588">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="589" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A589" t="s">
+        <v>165</v>
+      </c>
+      <c r="B589" t="s">
+        <v>621</v>
+      </c>
+      <c r="C589" t="s">
+        <v>498</v>
+      </c>
+      <c r="D589" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E589">
+        <v>0</v>
+      </c>
+      <c r="F589">
+        <v>0</v>
+      </c>
+      <c r="G589">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="590" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A590" t="s">
+        <v>166</v>
+      </c>
+      <c r="B590" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="591" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A591" t="s">
+        <v>167</v>
+      </c>
+      <c r="B591" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="592" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A592" t="s">
+        <v>168</v>
+      </c>
+      <c r="B592" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="593" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A593" t="s">
+        <v>169</v>
+      </c>
+      <c r="B593" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="594" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A594" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B594" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="595" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A595" t="s">
+        <v>171</v>
+      </c>
+      <c r="B595" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A596" t="s">
+        <v>172</v>
+      </c>
+      <c r="B596" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A597" t="s">
+        <v>173</v>
+      </c>
+      <c r="B597" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="598" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A598" t="s">
+        <v>174</v>
+      </c>
+      <c r="B598" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="599" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A599" t="s">
+        <v>175</v>
+      </c>
+      <c r="B599" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="600" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A600" t="s">
         <v>176</v>
       </c>
-      <c r="B512" t="s">
+      <c r="B600" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="513" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A513" t="s">
+    <row r="601" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A601" t="s">
         <v>177</v>
       </c>
-      <c r="B513" t="s">
+      <c r="B601" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="514" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A514" t="s">
+    <row r="602" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A602" t="s">
         <v>178</v>
       </c>
-      <c r="B514" t="s">
+      <c r="B602" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="515" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A515" t="s">
+    <row r="603" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A603" t="s">
         <v>179</v>
       </c>
-      <c r="B515" t="s">
+      <c r="B603" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="516" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A516" t="s">
+    <row r="604" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A604" t="s">
         <v>180</v>
       </c>
-      <c r="B516" t="s">
+      <c r="B604" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="517" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A517" t="s">
+    <row r="605" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A605" t="s">
         <v>181</v>
       </c>
-      <c r="B517" t="s">
+      <c r="B605" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="518" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A518" t="s">
+    <row r="606" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A606" t="s">
         <v>182</v>
       </c>
-      <c r="B518" t="s">
+      <c r="B606" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="519" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A519" t="s">
+    <row r="607" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A607" t="s">
         <v>183</v>
       </c>
-      <c r="B519" t="s">
+      <c r="B607" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="520" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A520" t="s">
+    <row r="608" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A608" t="s">
         <v>184</v>
       </c>
-      <c r="B520" t="s">
+      <c r="B608" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="521" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A521" t="s">
+    <row r="609" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A609" t="s">
         <v>185</v>
       </c>
     </row>

</xml_diff>

<commit_message>
arregle nombre cientifico de ostra del pacifico
</commit_message>
<xml_diff>
--- a/information/raw_databases/ADUANAS_CHILE/arancel_aduanero_nomenclatura/arancel_aduanero_2017/codigos_aduana_por_especie_2017.xlsx
+++ b/information/raw_databases/ADUANAS_CHILE/arancel_aduanero_nomenclatura/arancel_aduanero_2017/codigos_aduana_por_especie_2017.xlsx
@@ -2792,7 +2792,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2847,13 +2847,6 @@
       <name val="Times New Roman"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -2897,7 +2890,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -2913,7 +2906,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -3241,8 +3233,8 @@
   <dimension ref="A1:G609"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A551" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H573" sqref="H573"/>
+      <pane ySplit="1" topLeftCell="A557" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B608" sqref="B608"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13380,7 +13372,7 @@
         <v>560</v>
       </c>
       <c r="B441" t="s">
-        <v>561</v>
+        <v>777</v>
       </c>
       <c r="C441" t="s">
         <v>777</v>
@@ -13403,7 +13395,7 @@
         <v>560</v>
       </c>
       <c r="B442" t="s">
-        <v>561</v>
+        <v>777</v>
       </c>
       <c r="C442" t="s">
         <v>777</v>
@@ -13426,7 +13418,7 @@
         <v>560</v>
       </c>
       <c r="B443" t="s">
-        <v>561</v>
+        <v>777</v>
       </c>
       <c r="C443" t="s">
         <v>777</v>
@@ -14020,13 +14012,13 @@
       </c>
     </row>
     <row r="469" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A469" s="13" t="s">
+      <c r="A469" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="B469" s="13" t="s">
+      <c r="B469" s="12" t="s">
         <v>575</v>
       </c>
-      <c r="C469" s="13" t="s">
+      <c r="C469" s="12" t="s">
         <v>575</v>
       </c>
       <c r="D469" s="6" t="s">
@@ -16412,7 +16404,7 @@
       </c>
     </row>
     <row r="573" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A573" s="12" t="s">
+      <c r="A573" s="4" t="s">
         <v>150</v>
       </c>
       <c r="B573" t="s">

</xml_diff>